<commit_message>
Fix: Chapter 1 & 2, Reset
</commit_message>
<xml_diff>
--- a/Build/Signal-Lost-Chapters.xlsx
+++ b/Build/Signal-Lost-Chapters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\Games\Visual Studio 2022\C++\Signal-Lost\Signal-Lost\Build\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CE0FD7-4BF2-453C-95E9-A942A247B335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187E240C-113A-4E5A-BAA4-055593E0E6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters Header" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="349">
   <si>
     <t>Chapter Name</t>
   </si>
@@ -154,11 +154,6 @@
   <si>
     <t>[Choice1=[NextScene=2][Content=Pick it up.]]
 [Choice2=[Default=True][NextScene=3][Content=Hang up.]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextChapter=1][NextScene=1][Content=Retry.]]
-[Choice2=[Menu=True][Content=Menu.]]
-[Choice3=[Quit=True][Content=Quit.]]</t>
   </si>
   <si>
     <t>[Choice1=[NextScene=7][Content=Yeah, I think so?]]</t>
@@ -1312,6 +1307,355 @@
 I don't know when that thing was![Wait=500][Space=2]
 ...What?[Wait=500] I don't remember how I got here in the first place, don't expect me to remember this![Wait=500][Space=2]
 Anyway, you might want to search for that on the internet, it's a 4-digit password.[Wait=500] I'll try to log in.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=3][Content=Small?]]
+[Choice2=[NextScene=4][Content=Well preserved?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=13][Content=Why are you doubting all of a sudden?]]
+[Choice2=[NextScene=14][NextSceneNoTrust=13][TrustNeed=50][Content=Well, you might as well go and see inside to be sure!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=5][TrustAdd=25][Content=Nah. Why would someone want to clean an old museum anyway? It's a coincidence.]]
+[Choice2=[NextScene=6][Content=I guess there is, why would it be cleaner than the other building otherwise?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=6][Content=You're afraid of seeing someone now?]]
+[Choice2=[NextScene=7][TrustAdd=-25][Content=Well, don't enter it then.]]
+[Choice3=[NextScene=8][Content=Sorry to announce that, but it doesn't seem that you have the choice...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=8][TrustAdd=25][Content=Everything's gonna be fine as long as we collaborate.]]
+[Choice2=[NextScene=9][TrustAdd=-25][Content=I knew it! You're chicken-hearted!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=8][TrustAdd=25][Content=You're not in danger as long as I'm with you!]]
+[Choice2=[NextScene=9][Content=I knew you were chicken-hearted!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=Is there something weird in here?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=10][TrustAdd=-25][Content=Shhhh!! What if there's really someone here?]]
+[Choice2=[NextScene=11][Content=That's more like it!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=What makes you feel like that?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=12][TrustAdd=25][Content=Well... I am]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=What about it?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=6][Content=You're afraid of seeing someone now?]]
+[Choice2=[NextScene=7][TrustAdd=-25][Content=Well, don't enter it then.]]
+[Choice3=[NextScene=8][Content=Sorry to announce that, but it doesn't seem that you have the choice...]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=So? What's inside?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=16][Content=That's weird...]]
+[Choice2=[NextScene=17][TrustAdd=-25][Content=That's so cool!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=18][TrustAdd=-25][Content=You're becoming paranoïd?]]
+[Choice2=[NextScene=19][Content=Someone's living here?]]
+[Choice3=[NextScene=20][TrustAdd=25][Content=That we have a new mystery to resolve!]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=18][TrustAdd=-25][Content=You're definitly becoming paranoïd.]]
+[Choice2=[NextScene=19][Content=Is... someone living here?]]
+[Choice3=[NextScene=20][TrustAdd=25][Content=Seems that we'll have to solve this mystery together!]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=21][TrustAdd=-25][Content=I think I would be braver than you!]]
+[Choice2=[NextScene=22][TrustAdd=25][Content=I think I'd manage things like you.]]
+[Choice3=[NextScene=23][Content=I'd be... more fearful than you!]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=24][TrustAdd=25][Content=Calm Down. That doesn't justify any panic.]]
+[Choice2=[NextScene=25][TrustAdd=-25][Content=Don't throw up on the art please.]]
+[Choice3=[NextScene=26][TrustAdd=-25][Content=I was joking around! There's surely not anyone here.]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=27][Content=What is around you again?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=28][Content=Go and see the paintings.]]
+[Choice2=[NextScene=29][Content=Go and see the sculpture.]]
+[Choice3=[NextScene=30][Content=Go and see the inscriptions on the rock.]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=31][Content=Is there something else than art here?]]
+[Choice2=[NextScene=39][Content=Can you describe it more precisely?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=31][Content=Is there something else than art here?]]
+[Choice2=[NextScene=40][Content=Can you describe it more precisely?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=31][Content=Is there something else than art here?]]
+[Choice2=[NextScene=41][Content=Can you describe it more precisely?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=32][Content=What's going on?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=33][Content=It must be a secret escape!]]
+[Choice2=[NextScene=33][Content=Watch out, it might be trapped.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=34][Content=Can you read it for me?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=35][Content=What is there in the museum again?]]
+[Choice2=[NextScene=45][Content=I think I might have an idea for the code.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=34][Content=Can I see the note again?]]
+[Choice2=[NextScene=36][Content=Go and see the paintings.]]
+[Choice3=[NextScene=37][Content=Go and see the sculpture.]]
+[Choice4=[NextScene=38][Content=Go and see the inscriptions on the rock.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=42][Content=Can I have more information about it?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=43][Content=Can I have more information about it?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=44][Content=Can I have more information about it?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=27][Content=What else is here?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=35][Content=Can you say again what's in here?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=35][Content=Wait... Can we just check the museum again?]]
+[Choice2=[NextScene=46][Content=Hell yeah, show me this keypad!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=49][Content=A.]]
+[Choice2=[NextScene=47][Content=L.]]
+[Choice3=[NextScene=49][Content=O.]]
+[Choice4=[NextScene=49][Content=P.]]
+[Choice5=[NextScene=49][Content=S.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=49][Content=D.]]
+[Choice2=[NextScene=48][Content=G.]]
+[Choice3=[NextScene=49][Content=L.]]
+[Choice4=[NextScene=49][Content=W.]]
+[Choice5=[NextScene=49][Content=Y.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=52][Content=C.]]
+[Choice2=[NextScene=49][Content=E.]]
+[Choice3=[NextScene=49][Content=R.]]
+[Choice4=[NextScene=49][Content=S.]]
+[Choice5=[NextScene=49][Content=U.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=50][Content=You have to get out!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=51][Content=Are you here?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextChapter=2][Reset=True][NextScene=1][Content=Retry.]]
+[Choice2=[NextChapter=1][Reset=True][NextScene=1][Content=Retry from Chapter-1.]]
+[Choice3=[Menu=True][Content=Menu.]]
+[Choice4=[Quit=True][Content=Quit.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextChapter=1][Reset=True][NextScene=1][Content=Retry.]]
+[Choice2=[Menu=True][Content=Menu.]]
+[Choice3=[Quit=True][Content=Quit.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=53][Content=What are you expecting to find here?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=54][Content=What if you don't find any fuse?]]
+[Choice2=[NextScene=58][Content=What if there was someone down there?]]
+[Choice3=[NextScene=61][Content=What if it's a trap?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=55][TrustAdd=25][Content=Of course! I will be with you until the end.]]
+[Choice2=[NextScene=56][TrustAdd=-25][Content=Uhm, I have more alluring stuff to do.]]
+[Choice3=[NextScene=57][TrustAdd=25][Content=Sorry but I don't feel confortable with hearing someone slowly dying on phone...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=64][Content=I was just being honest! You're down the stairs?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=64][Content=It's cool to see that you understand! You're down the stairs?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=64][Content=Funny one. You're down the stairs?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=59][TrustAdd=-25][Content=But they'll be hostile!]]
+[Choice2=[NextScene=60][Content=Maybe we can deal so they free you.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=64][Content=Where ar you now?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=62][TrustAdd=-25][Content=I would go back and search for another way out if I were you.]]
+[Choice2=[NextScene=63][Content=Do whatever you want, it's your responsability.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=64][Content=So you're getting down there?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=64][Content=I'll do my best... Where are you now?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=65][Content=Shit! The signal's getting weaker again!]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Choice1=[NextScene=66][Content=Can you hear me?]]
+[Choice2=[NextScene=66][Content=I'm still here!]]
+</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=67][Content=Who is this?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=68][Content=How do I know I can trust you?]]
+[Choice2=[NextScene=69][Content=What should I do?!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=69][Content=Okay, tell me how I can help.]]
+[Choice2=[NextScene=69][Content=I won't listen to you!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=70][Content=I'm ready.]]
+[Choice2=[NextScene=70][Content=Questions? And how is it going to help?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=71][TrustAdd=25][Content=Yes.]]
+[Choice2=[NextScene=71][TrustAdd=-25][Content=No.]]
+[Choice3=[Default=True][NextScene=71][TrustAdd=-25][Content=How can I answer that?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=72][TrustAdd=25][Content=Yes?]]
+[Choice2=[NextScene=72][TrustAdd=25][Content=No?]]
+[Choice3=[Default=True][NextScene=72][TrustAdd=-25][Content=But that's impossible?!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=73][TrustAdd=25][Content=Yes!]]
+[Choice2=[NextScene=73][TrustAdd=-25][Content=No!]]
+[Choice3=[Default=True][NextScene=73][TrustAdd=-25][Content=I would worry about getting out instead of doing small talk!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=74][Content=Yes!]]
+[Choice2=[NextScene=75][Content=Something crazy just happened...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=75][NextSceneNoTrust=77][TrustNeed=75][Content=I was.]]
+[Choice2=[NextScene=76][TrustAdd=-25][Content=I was not.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=78][Content=I have no idea!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=79][Content=HIDE!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=80][Content=Who is this?]]
+[Choice2=[NextScene=80][Content=Don't say a word!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=81][Content=DON'T TALK TO HIM!]]
+[Choice2=[NextScene=81][Content=Is this the one who put you on this island?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=82][Content=Y-You're a clone of me?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=83][Content=He's lying!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=84][Content=That's a good question!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=85][Content=All the clones before died?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=86][Content=Virus? Immune?]]
+[Choice2=[NextScene=86][Content=Is that the one who contacted me earlier? Or was it you?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=87][Content=Calm down!]]
+[Choice2=[NextScene=87][Content=That's it! Why did you clone me?!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=88][Content=Yes! Why should we trust you?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=89][Content=AND WHY WOULD YOU CHOOSE ME?!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=90][Content=IT'S ALL A LIE! STAY INSIDE!]]
+[Choice2=[NextScene=100][NextSceneNoTrust=93][TrustNeed=75][Content=Follow him...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=91][Content=What is this noise?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=92][Content=DONT GIVE UP!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=94][Content=You're getting everything wrong!]]
+[Choice2=[NextScene=95][Content=Why are you acting like this?!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=95][Content=I'm not!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=96][Content=You're losing your mind.]]
+[Choice2=[NextScene=96][Content=Come back to your senses!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=97][Content=DON'T DO THAT! You'll get killed!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=98][Content=You're really dumb.]]
+[Choice2=[NextScene=98][Content=STOP THAT!]]
+[Choice3=[NextScene=100][Content=I'VE GOT NOTHING TO DO WITH THIS!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=99][Content=You're getting everything wrong!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=101][Content=That's reassuring!]]
+[Choice2=[NextScene=102][Content=That might be the worst thing to say to put someone at ease.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=103][Content=That's...]]
+[Choice2=[NextScene=103][Content=It is...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=104][Content=That was quite an adventure!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=105][Content=You are more than just an alternate version of me!]]
+[Choice2=[NextScene=105][Content=It's you that will save the world in the end, not me.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=106][Content=We'll go and see a movie too! Since your favorites one are also mine.]]
+[Choice2=[NextScene=106][Content=I hope you don't remember the awkward ones...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=107][Content=See you later.]]</t>
   </si>
 </sst>
 </file>
@@ -1744,13 +2088,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1785,6 +2122,13 @@
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2927,45 +3271,45 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{06011938-0AD2-4BD5-94CE-F0E0A0E0FFA3}" name="Tableau24" displayName="Tableau24" ref="A1:F108" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{06011938-0AD2-4BD5-94CE-F0E0A0E0FFA3}" name="Tableau24" displayName="Tableau24" ref="A1:F108" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="A1:F108" xr:uid="{06011938-0AD2-4BD5-94CE-F0E0A0E0FFA3}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B6918237-504D-4F26-A222-E23222E5B942}" name="Scene Number" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{F64899E5-1A64-49E6-A65F-EAAE71EE5915}" name="Beep Background" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{BC5F93A0-4B65-407D-8D72-4A595DDB1B1A}" name="Connexion" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{4E0A9704-4921-4E7C-9AEB-FB20BB4EC8A3}" name="Timer (s)" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{43982405-9B08-4755-AFD4-0248FE69AD29}" name="Content" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{D6735575-D999-4E9F-B6E6-A37C953B1751}" name="Choices" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B6918237-504D-4F26-A222-E23222E5B942}" name="Scene Number" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{F64899E5-1A64-49E6-A65F-EAAE71EE5915}" name="Beep Background" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{BC5F93A0-4B65-407D-8D72-4A595DDB1B1A}" name="Connexion" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{4E0A9704-4921-4E7C-9AEB-FB20BB4EC8A3}" name="Timer (s)" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{43982405-9B08-4755-AFD4-0248FE69AD29}" name="Content" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{D6735575-D999-4E9F-B6E6-A37C953B1751}" name="Choices" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{38B76A2D-5C14-428E-A8D7-2AB25FA6F09C}" name="Tableau245" displayName="Tableau245" ref="A1:F74" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{38B76A2D-5C14-428E-A8D7-2AB25FA6F09C}" name="Tableau245" displayName="Tableau245" ref="A1:F74" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="A1:F74" xr:uid="{38B76A2D-5C14-428E-A8D7-2AB25FA6F09C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2D0CA42B-42CD-4F28-A244-F6A74F1D49EB}" name="Scene Number" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{EF2DE2AD-F265-4A83-8AC6-2041CA7A8BC0}" name="Beep Background" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{60D7AEA9-B919-463B-9AFA-B4883B9ED875}" name="Connexion" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{218C9B1B-386E-4AB7-84BD-7528C8622B41}" name="Timer (s)" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{93695F6A-E1B4-44DB-9850-1E0D3CB2763F}" name="Content" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{05D2F5DC-4A0C-489B-8CEB-B5E67AE224DB}" name="Choices" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{2D0CA42B-42CD-4F28-A244-F6A74F1D49EB}" name="Scene Number" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{EF2DE2AD-F265-4A83-8AC6-2041CA7A8BC0}" name="Beep Background" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{60D7AEA9-B919-463B-9AFA-B4883B9ED875}" name="Connexion" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{218C9B1B-386E-4AB7-84BD-7528C8622B41}" name="Timer (s)" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{93695F6A-E1B4-44DB-9850-1E0D3CB2763F}" name="Content" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{05D2F5DC-4A0C-489B-8CEB-B5E67AE224DB}" name="Choices" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{294BB542-FB8B-4889-B6DC-CCE42BDEC50A}" name="Tableau246" displayName="Tableau246" ref="A1:F74" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{294BB542-FB8B-4889-B6DC-CCE42BDEC50A}" name="Tableau246" displayName="Tableau246" ref="A1:F74" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A1:F74" xr:uid="{294BB542-FB8B-4889-B6DC-CCE42BDEC50A}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{86A45CC4-D1E4-4189-A0E3-6B34C1221E8C}" name="Scene Number" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{B358CBDC-D578-4810-A1FA-D4DF86435BB2}" name="Beep Background" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{15BA870F-AE75-4AD1-B763-10D71A428A1B}" name="Connexion" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{16411923-4C65-4B77-B018-045BA2C5B364}" name="Timer (s)" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{38F12D75-BEA7-4F52-89D6-940D9240151E}" name="Content" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{63721DBF-8860-4EE4-ABCF-6CE35DD2BB70}" name="Choices" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{86A45CC4-D1E4-4189-A0E3-6B34C1221E8C}" name="Scene Number" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B358CBDC-D578-4810-A1FA-D4DF86435BB2}" name="Beep Background" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{15BA870F-AE75-4AD1-B763-10D71A428A1B}" name="Connexion" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{16411923-4C65-4B77-B018-045BA2C5B364}" name="Timer (s)" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{38F12D75-BEA7-4F52-89D6-940D9240151E}" name="Content" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{63721DBF-8860-4EE4-ABCF-6CE35DD2BB70}" name="Choices" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3287,7 +3631,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="12">
         <v>3</v>
@@ -3304,7 +3648,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="12">
         <v>3</v>
@@ -3321,7 +3665,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="12">
         <v>3</v>
@@ -3345,8 +3689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView topLeftCell="E37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="120" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3392,7 +3736,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>29</v>
@@ -3408,7 +3752,7 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>12</v>
@@ -3424,10 +3768,10 @@
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>30</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3438,7 +3782,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>26</v>
@@ -3452,7 +3796,7 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>27</v>
@@ -3468,10 +3812,10 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3484,10 +3828,10 @@
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3501,7 +3845,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3512,10 +3856,10 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3526,10 +3870,10 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>215</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3540,10 +3884,10 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3554,10 +3898,10 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3571,7 +3915,7 @@
         <v>19</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3582,10 +3926,10 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3613,7 +3957,7 @@
         <v>20</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3627,7 +3971,7 @@
         <v>21</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3641,7 +3985,7 @@
         <v>22</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3655,7 +3999,7 @@
         <v>23</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3669,7 +4013,7 @@
         <v>24</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3680,10 +4024,10 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3696,10 +4040,10 @@
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3712,10 +4056,10 @@
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>30</v>
+        <v>299</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3731,7 +4075,7 @@
         <v>14</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3744,10 +4088,10 @@
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>30</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3758,10 +4102,10 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3774,10 +4118,10 @@
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3788,10 +4132,10 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3802,10 +4146,10 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3816,10 +4160,10 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3830,10 +4174,10 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3844,10 +4188,10 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3858,10 +4202,10 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3872,10 +4216,10 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3886,10 +4230,10 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3902,10 +4246,10 @@
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3918,10 +4262,10 @@
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3932,10 +4276,10 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3946,10 +4290,10 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3960,10 +4304,10 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3974,10 +4318,10 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3988,10 +4332,10 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4002,10 +4346,10 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4016,10 +4360,10 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4030,10 +4374,10 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4044,10 +4388,10 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4058,10 +4402,10 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4072,10 +4416,10 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4086,10 +4430,10 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4100,10 +4444,10 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4114,10 +4458,10 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4132,10 +4476,10 @@
         <v>60</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4148,10 +4492,10 @@
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4164,10 +4508,10 @@
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>30</v>
+        <v>299</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4183,7 +4527,7 @@
         <v>15</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4196,10 +4540,10 @@
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4210,10 +4554,10 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4224,10 +4568,10 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4238,10 +4582,10 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4252,10 +4596,10 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4266,10 +4610,10 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4280,10 +4624,10 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4294,10 +4638,10 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4308,10 +4652,10 @@
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4322,10 +4666,10 @@
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4339,7 +4683,7 @@
         <v>16</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4352,10 +4696,10 @@
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4368,10 +4712,10 @@
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4382,10 +4726,10 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4396,10 +4740,10 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4410,10 +4754,10 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4426,10 +4770,10 @@
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4443,7 +4787,7 @@
         <v>17</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -4459,8 +4803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305A82C4-79AC-4307-9167-395B8B5B112C}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="E103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="120" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4502,10 +4846,10 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4516,9 +4860,11 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="8"/>
+        <v>95</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -4528,9 +4874,11 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" s="8"/>
+        <v>96</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -4540,9 +4888,11 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="8"/>
+        <v>97</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -4552,9 +4902,11 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="8"/>
+        <v>98</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -4564,9 +4916,11 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="8"/>
+        <v>99</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -4576,9 +4930,11 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="F8" s="8"/>
+        <v>100</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -4588,9 +4944,11 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F9" s="8"/>
+        <v>144</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -4600,9 +4958,11 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F10" s="8"/>
+        <v>145</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -4612,9 +4972,11 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="F11" s="8"/>
+        <v>101</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -4624,9 +4986,11 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="F12" s="8"/>
+        <v>146</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -4636,9 +5000,11 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -4648,9 +5014,11 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" s="8"/>
+        <v>103</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -4660,9 +5028,11 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F15" s="8"/>
+        <v>147</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -4672,9 +5042,11 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" s="8"/>
+        <v>104</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -4684,9 +5056,11 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F17" s="8"/>
+        <v>105</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -4696,9 +5070,11 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="8"/>
+        <v>106</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
@@ -4708,9 +5084,11 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19" s="8"/>
+        <v>107</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -4720,9 +5098,11 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F20" s="8"/>
+        <v>148</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -4732,9 +5112,11 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="8"/>
+        <v>108</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
@@ -4744,9 +5126,11 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="8"/>
+        <v>109</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -4756,9 +5140,11 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F23" s="8"/>
+        <v>110</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -4768,9 +5154,11 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F24" s="8"/>
+        <v>111</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -4780,9 +5168,11 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="F25" s="8"/>
+        <v>149</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -4792,9 +5182,11 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="F26" s="8"/>
+        <v>150</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
@@ -4804,9 +5196,11 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" s="8"/>
+        <v>112</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
@@ -4816,9 +5210,11 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="F28" s="8"/>
+        <v>113</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -4828,9 +5224,11 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="F29" s="8"/>
+        <v>151</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -4840,9 +5238,11 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F30" s="8"/>
+        <v>152</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
@@ -4852,9 +5252,11 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="F31" s="8"/>
+        <v>153</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
@@ -4864,9 +5266,11 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F32" s="8"/>
+        <v>154</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
@@ -4876,9 +5280,11 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="F33" s="8"/>
+        <v>114</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
@@ -4888,9 +5294,11 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="F34" s="8"/>
+        <v>155</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
@@ -4900,9 +5308,11 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="F35" s="8"/>
+        <v>156</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
@@ -4912,9 +5322,11 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F36" s="8"/>
+        <v>117</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
@@ -4924,9 +5336,11 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="F37" s="8"/>
+        <v>151</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
@@ -4936,9 +5350,11 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F38" s="8"/>
+        <v>152</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
@@ -4948,9 +5364,11 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="F39" s="8"/>
+        <v>153</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
@@ -4960,9 +5378,11 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F40" s="8"/>
+        <v>118</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
@@ -4972,9 +5392,11 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="F41" s="8"/>
+        <v>119</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -4984,9 +5406,11 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="F42" s="8"/>
+        <v>157</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -4996,9 +5420,11 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F43" s="8"/>
+        <v>118</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -5008,9 +5434,11 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="F44" s="8"/>
+        <v>119</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
@@ -5020,9 +5448,11 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="F45" s="8"/>
+        <v>157</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
@@ -5032,9 +5462,11 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F46" s="8"/>
+        <v>120</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
@@ -5044,9 +5476,11 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="F47" s="8"/>
+        <v>160</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="48" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -5056,9 +5490,11 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="F48" s="8"/>
+        <v>158</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
@@ -5068,9 +5504,11 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="F49" s="8"/>
+        <v>159</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="50" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
@@ -5082,9 +5520,11 @@
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="F50" s="8"/>
+        <v>161</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="51" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
@@ -5096,9 +5536,11 @@
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="F51" s="8"/>
+        <v>162</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
@@ -5110,9 +5552,11 @@
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="F52" s="8"/>
+        <v>204</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -5122,9 +5566,11 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F53" s="8"/>
+        <v>163</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="54" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -5134,9 +5580,11 @@
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="F54" s="8"/>
+        <v>122</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -5146,9 +5594,11 @@
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="F55" s="8"/>
+        <v>123</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="56" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
@@ -5158,9 +5608,11 @@
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="F56" s="8"/>
+        <v>124</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -5170,9 +5622,11 @@
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="F57" s="8"/>
+        <v>125</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
@@ -5182,9 +5636,11 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="F58" s="8"/>
+        <v>126</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="59" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -5194,9 +5650,11 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F59" s="8"/>
+        <v>127</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="60" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
@@ -5206,9 +5664,11 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="F60" s="8"/>
+        <v>128</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="61" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
@@ -5218,9 +5678,11 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F61" s="8"/>
+        <v>129</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="62" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
@@ -5230,9 +5692,11 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F62" s="8"/>
+        <v>130</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="63" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
@@ -5242,9 +5706,11 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="F63" s="8"/>
+        <v>131</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="64" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
@@ -5254,9 +5720,11 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="F64" s="8"/>
+        <v>132</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="65" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
@@ -5268,9 +5736,11 @@
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="F65" s="8"/>
+        <v>164</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="66" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
@@ -5282,9 +5752,11 @@
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="F66" s="8"/>
+        <v>165</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="67" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
@@ -5294,9 +5766,11 @@
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="F67" s="8"/>
+        <v>175</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="68" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
@@ -5306,9 +5780,11 @@
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="F68" s="8"/>
+        <v>176</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="69" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
@@ -5318,9 +5794,11 @@
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="F69" s="8"/>
+        <v>177</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="70" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
@@ -5330,9 +5808,11 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="F70" s="8"/>
+        <v>178</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="71" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
@@ -5344,9 +5824,11 @@
         <v>7</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="F71" s="8"/>
+        <v>179</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="72" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
@@ -5358,9 +5840,11 @@
         <v>7</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="F72" s="8"/>
+        <v>180</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="73" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
@@ -5372,9 +5856,11 @@
         <v>7</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="F73" s="8"/>
+        <v>181</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="74" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10">
@@ -5384,9 +5870,11 @@
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="F74" s="13"/>
+        <v>182</v>
+      </c>
+      <c r="F74" s="13" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="75" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="10">
@@ -5398,9 +5886,11 @@
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="F75" s="13"/>
+        <v>135</v>
+      </c>
+      <c r="F75" s="13" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="76" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="10">
@@ -5410,9 +5900,11 @@
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
       <c r="E76" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F76" s="13"/>
+        <v>133</v>
+      </c>
+      <c r="F76" s="13" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="77" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="10">
@@ -5422,9 +5914,11 @@
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
       <c r="E77" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F77" s="13"/>
+        <v>134</v>
+      </c>
+      <c r="F77" s="13" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="78" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10">
@@ -5434,9 +5928,11 @@
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
       <c r="E78" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="F78" s="13"/>
+        <v>136</v>
+      </c>
+      <c r="F78" s="13" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="79" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="10">
@@ -5446,9 +5942,11 @@
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
       <c r="E79" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="F79" s="13"/>
+        <v>166</v>
+      </c>
+      <c r="F79" s="13" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="80" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="10">
@@ -5458,9 +5956,11 @@
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
       <c r="E80" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="F80" s="13"/>
+        <v>167</v>
+      </c>
+      <c r="F80" s="13" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="81" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="10">
@@ -5470,9 +5970,11 @@
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
       <c r="E81" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="F81" s="13"/>
+        <v>168</v>
+      </c>
+      <c r="F81" s="13" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="82" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="10">
@@ -5482,9 +5984,11 @@
       <c r="C82" s="12"/>
       <c r="D82" s="12"/>
       <c r="E82" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="F82" s="13"/>
+        <v>169</v>
+      </c>
+      <c r="F82" s="13" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="83" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10">
@@ -5494,9 +5998,11 @@
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
       <c r="E83" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="F83" s="13"/>
+        <v>170</v>
+      </c>
+      <c r="F83" s="13" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="84" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="10">
@@ -5506,9 +6012,11 @@
       <c r="C84" s="12"/>
       <c r="D84" s="12"/>
       <c r="E84" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="F84" s="13"/>
+        <v>171</v>
+      </c>
+      <c r="F84" s="13" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="85" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10">
@@ -5518,9 +6026,11 @@
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
       <c r="E85" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="F85" s="13"/>
+        <v>172</v>
+      </c>
+      <c r="F85" s="13" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="86" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="10">
@@ -5530,9 +6040,11 @@
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
       <c r="E86" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="F86" s="13"/>
+        <v>173</v>
+      </c>
+      <c r="F86" s="13" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="87" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="10">
@@ -5542,9 +6054,11 @@
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
       <c r="E87" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="F87" s="13"/>
+        <v>174</v>
+      </c>
+      <c r="F87" s="13" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="88" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="10">
@@ -5554,9 +6068,11 @@
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
       <c r="E88" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="F88" s="13"/>
+        <v>183</v>
+      </c>
+      <c r="F88" s="13" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="89" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="10">
@@ -5566,9 +6082,11 @@
       <c r="C89" s="12"/>
       <c r="D89" s="12"/>
       <c r="E89" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="F89" s="13"/>
+        <v>184</v>
+      </c>
+      <c r="F89" s="13" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="90" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="10">
@@ -5578,9 +6096,11 @@
       <c r="C90" s="12"/>
       <c r="D90" s="12"/>
       <c r="E90" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="F90" s="13"/>
+        <v>185</v>
+      </c>
+      <c r="F90" s="13" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="91" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="10">
@@ -5592,9 +6112,11 @@
       </c>
       <c r="D91" s="12"/>
       <c r="E91" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="F91" s="13"/>
+        <v>186</v>
+      </c>
+      <c r="F91" s="13" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="92" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="10">
@@ -5606,9 +6128,11 @@
       </c>
       <c r="D92" s="12"/>
       <c r="E92" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="F92" s="13"/>
+        <v>187</v>
+      </c>
+      <c r="F92" s="13" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="93" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="10">
@@ -5620,9 +6144,11 @@
       </c>
       <c r="D93" s="12"/>
       <c r="E93" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="F93" s="13"/>
+        <v>203</v>
+      </c>
+      <c r="F93" s="13" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="94" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="10">
@@ -5634,9 +6160,11 @@
       </c>
       <c r="D94" s="12"/>
       <c r="E94" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="F94" s="13"/>
+        <v>189</v>
+      </c>
+      <c r="F94" s="13" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="95" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10">
@@ -5646,9 +6174,11 @@
       <c r="C95" s="12"/>
       <c r="D95" s="12"/>
       <c r="E95" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="F95" s="13"/>
+        <v>190</v>
+      </c>
+      <c r="F95" s="13" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="96" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10">
@@ -5658,9 +6188,11 @@
       <c r="C96" s="12"/>
       <c r="D96" s="12"/>
       <c r="E96" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F96" s="13"/>
+        <v>191</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="97" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10">
@@ -5670,9 +6202,11 @@
       <c r="C97" s="12"/>
       <c r="D97" s="12"/>
       <c r="E97" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="F97" s="13"/>
+        <v>192</v>
+      </c>
+      <c r="F97" s="13" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="98" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="10">
@@ -5682,9 +6216,11 @@
       <c r="C98" s="12"/>
       <c r="D98" s="12"/>
       <c r="E98" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="F98" s="13"/>
+        <v>193</v>
+      </c>
+      <c r="F98" s="13" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="99" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="10">
@@ -5696,9 +6232,11 @@
       </c>
       <c r="D99" s="12"/>
       <c r="E99" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="F99" s="13"/>
+        <v>194</v>
+      </c>
+      <c r="F99" s="13" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="100" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="10">
@@ -5710,9 +6248,11 @@
       </c>
       <c r="D100" s="12"/>
       <c r="E100" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="F100" s="13"/>
+        <v>202</v>
+      </c>
+      <c r="F100" s="13" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="101" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="10">
@@ -5724,9 +6264,11 @@
       </c>
       <c r="D101" s="12"/>
       <c r="E101" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="F101" s="13"/>
+        <v>195</v>
+      </c>
+      <c r="F101" s="13" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="102" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="10">
@@ -5736,9 +6278,11 @@
       <c r="C102" s="12"/>
       <c r="D102" s="12"/>
       <c r="E102" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="F102" s="13"/>
+        <v>197</v>
+      </c>
+      <c r="F102" s="13" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="103" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="10">
@@ -5748,9 +6292,11 @@
       <c r="C103" s="12"/>
       <c r="D103" s="12"/>
       <c r="E103" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="F103" s="13"/>
+        <v>196</v>
+      </c>
+      <c r="F103" s="13" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="104" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="10">
@@ -5760,9 +6306,11 @@
       <c r="C104" s="12"/>
       <c r="D104" s="12"/>
       <c r="E104" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="F104" s="13"/>
+        <v>198</v>
+      </c>
+      <c r="F104" s="13" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="105" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="10">
@@ -5772,9 +6320,11 @@
       <c r="C105" s="12"/>
       <c r="D105" s="12"/>
       <c r="E105" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="F105" s="13"/>
+        <v>199</v>
+      </c>
+      <c r="F105" s="13" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="106" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="10">
@@ -5784,9 +6334,11 @@
       <c r="C106" s="12"/>
       <c r="D106" s="12"/>
       <c r="E106" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="F106" s="13"/>
+        <v>200</v>
+      </c>
+      <c r="F106" s="13" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="107" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10">
@@ -5796,9 +6348,11 @@
       <c r="C107" s="12"/>
       <c r="D107" s="12"/>
       <c r="E107" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="F107" s="13"/>
+        <v>201</v>
+      </c>
+      <c r="F107" s="13" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="108" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="10">
@@ -5810,9 +6364,11 @@
       </c>
       <c r="D108" s="12"/>
       <c r="E108" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="F108" s="13"/>
+        <v>207</v>
+      </c>
+      <c r="F108" s="13" t="s">
+        <v>298</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix: Chapters 1 & 2
</commit_message>
<xml_diff>
--- a/Build/Signal-Lost-Chapters.xlsx
+++ b/Build/Signal-Lost-Chapters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\Games\Visual Studio 2022\C++\Signal-Lost\Signal-Lost\Build\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4561932-6C04-4AF5-852F-AEBECFBE7EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65542DEB-B14B-47F5-BCBB-6A048AE01623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="350">
   <si>
     <t>Chapter Name</t>
   </si>
@@ -402,109 +402,8 @@
     <t>The Factory</t>
   </si>
   <si>
-    <t>Going to the museum?[Wait=500] I can work with that.[Wait=500][Space=2]
-This whole trapdoor thing is supicious anyway.[Wait=500] It might be better to explore this place before doing anything stupid.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>It's not that far away, I think I can even see it from here![Wait=500] I'll take you back in a second when I'll be there![Wait=500][Space=2]
-.[Wait=500].[Wait=500].[Wait=500][Space=2]
-.[Wait=500].[Wait=500].[Wait=500][Space=2]
-Okay![Wait=500] I'm in front of it.[Wait=500] It's smaller than I thought, and it looks really well preserved![Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>It looks like this place has only one big main room inside.[Wait=500][Space=2]
 I don't know if there'll be anything interesting here...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>That's weird right?[Wait=500][Space=2]
-All this place has is empty buildings withered by the time.[Wait=500][Space=2]
-It's weird that a useless building is still standing unharmed.[Wait=500][Space=2]
-...[Wait=500] Does that mean that someone's still here to assure this museum is clean?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>I'm sure you're right...[Wait=500] But it feels odd, still.[Wait=500][Space=2]
-I'm great.[Wait=500] Now I don't feel like entering this place.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>I guess I am...[Wait=500] The fact that everything seems to be designed to make me explore this place is...[Wait=500][Space=2]
-Yes, I'm scared...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>I FEEL like not entering, but I have no choice and I think you know it well![Wait=500][Space=2]
-I-...[Wait=500] I could do that but there's nothing that could help me escape that strikes my mind.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>What did I hear?[Wait=500] Is someone getting scared all of the sudden?[Wait=500] That'll teach you![Wait=500][Space=2]
-But there doesn't seem to be anyone here anyway.[Wait=500][Space=2]
-Looks like we both worried for nothing.[Wait=500][Space=2]
-...[Wait=500] But there still somthing off-putting here.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>That's fair, but you seem like a good guy.[Wait=500][Space=2]
-I'm not going to be scared by a voice coming from an old flipphone![Wait=500][Space=2]
-But let's focus more on this museum now.[Wait=500] Something's off.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>...[Wait=500] I don't think going inside the only building that looks inhabited is a good idea.[Wait=500][Space=2]
-I don't want to land face to face with someone hostile.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>The inside of this museum truly feels abnormal...[Wait=500][Space=2]
-Everything's clean, there's not a single bit of dust here![Wait=500][Space=2]
-All these paintings are perfectly displayed,[Wait=500] sculptures are bright polished...[Wait=500][Space=2]
-There's even historical relics preserved under glass bells![Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>It definitly![Wait=500] How can this museum be this clean?[Wait=500][Space=2]
-Considering that it's the first time I see a place not post-apocalyptic-looking on this island...[Wait=500][Space=2]
-It surely means that...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>...[Wait=500] No, it isn't?[Wait=500][Space=2]
-It's unsettling...[Wait=500] Every place I've been through on this island has only been ruins and now that![Wait=500][Space=2]
-It most defintly means that this place is special somehow...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>...[Wait=500] What?[Wait=500] Wouldn't you be paranoïd after going through what I'm living?[Wait=500][Space=2]
-I'd like us to switch place and see how you could manage all this...[Wait=500][Space=2]
-How would you like that idea?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>...[Wait=500] I didn't expected that kind of answer but it feels weirdly refreshing![Wait=500][Space=2]
-It's nice having someone dedramatizing this whole situation.[Wait=500][Space=2]
-Let's go and solve that mystery then! Where should I go?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>That's a bold thing to say![Wait=500][Space=2]
-You're really are a daredevil huh?[Wait=500][Space=2]
-Well I'm not, and you'll have to bare with it.[Wait=500][Space=2]
-To refocus on what's important, I think exploring this room might be helpful.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>You see?[Wait=500] I guess we're not so different after all![Wait=500][Space=2]
-Now, this ideological question is interesting but it won't help me to escape from here, so let's explore this place![Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>AH![Wait=500] You get all showy while you couldn't handle a quarter of what I'm living![Wait=500][Space=2]
-...[Wait=500] I'm the one making fun of you but in the end I'm still the one stucked on this island...[Wait=500] Ironic.[Wait=500][Space=2]
-It might be the right time to come back at the main question : What is this place?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Well, I hope you're not a humorist![Wait=500][Space=2]
-You know it's really not the time to be joking around, right?[Wait=500][Space=2]
-I'm diving into the unknown and you think it's funny?[Wait=500] That's really irritating![Wait=500][Space=2]
-I don't want to argue here, so let's go see what this museum has to offer.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>There are paintings on the wall, from the impressionism era it seems.[Wait=500][Space=2]
-There's also all these sculptures of muscular men.[Wait=500] The greek heterocurious kind of sculpture, you know.[Wait=500][Space=2]
-And there's also these rock plates with strange language engraved on them.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>I-I don't know, the ground shaked for a second...[Wait=500][Space=2]
-Wait...[Wait=500] What's tha-...[Wait=500][Space=2]
-...Has a motherfucking door appeared at the back of the museum?[Wait=500][Space=2]
-Did I really activated a mechanism at random because of my rage?[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>Shhhh...[Wait=500][Space=2]
@@ -518,80 +417,20 @@
 Even if I don't think I can go fast enough to compete against this escalator eh![Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>There are paintings on the wall, from the impressionism era it seems.[Wait=500][Space=2]
-There's also all these sculptures of muscular men.[Wait=500] The greek heterocurious kind of sculpture, you know.[Wait=500][Space=2]
-There's also these rock plates with strange language engraved on them.[Wait=500][Space=2]
-And obviously this weird door with that letter keypad and the note.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>It's multiple painting picturing the same city it seems![Wait=500][Space=2]
-I can tell that because of the same looking monument one every of them.[Wait=500][Space=2]
-It's a huge white pillar with at the top a golden urn of fire, or something like that.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>It's a white statue of two men fighting.[Wait=500][Space=2]
-Well, I said two men but not really.[Wait=500] One is a centaur if I'm not mistaking.[Wait=500][Space=2]
-The human one is on top of him with a huge stick, ready to strike the centaur.[Wait=500][Space=2]
-That's a cool looking statue![Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Are you sure?[Wait=500] I don't know what could happen if I type the wrong code but I don't want to find out.[Wait=500][Space=2]
-You're confident?[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Hard to tell...[Wait=500] But I'm not going to lie, it's hard not to freak out about waking up on a random island...[Wait=500][Space=2]
 ...[Wait=500][Space=2]
 I-[Wait=500] Who knows what could be hiding in those buildings? Ha-[Wait=500] It’s hard to stay rational after what happened to me![Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>For now, all is see are stairs going deep down...[Wait=500][Space=2]
-But I hope that I'll found this fuse to activate the trapdoor in the outside.[Wait=500][Space=2]
-Or at least answers for why I'm here.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>That's not reassuring to say pal...[Wait=500][Space=2]
-What if there's no fuse?[Wait=500] Guess I'll die slowly, starving, while you're here listening to my agony.[Wait=500][Space=2]
-Would you be here to support here in my final moments?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Ahah![Wait=500] That was supposed to be a joke![Wait=500][Space=2]
-I admit  that I won't be able to handle that on side anyway.[Wait=500][Space=2]
-But if you're willing to hear me die, I guess that's okay![Wait=500] If that's not because of a twisted fantasy of yours...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Oh.[Wait=500] Uhm...[Wait=500][Space=2]
-Of course you have a life, I don't want to disturb you with my boring imminent death...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Ahah![Wait=500] Of course you're not![Wait=500] That was a joke![Wait=500][Space=2]
-Don't worry about it, if I ever find myself in this kind of situation, I don't you to suffer it too.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>...[Wait=500] If we put together the door system and the tidiness of this museum compared to the other buildings...[Wait=500][Space=2]
-Yes, I think I'm about to meet the ones responsible of all my troubles.[Wait=500][Space=2]
-I don't know what their project is, but I'm sure I'll soon find out if I speak directly to them.[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Don't you think that I considered this possibility?[Wait=500][Space=2]
 Of course they don't want me to go![Wait=500] But I have nothing to stop them other than trying to talk them out.[Wait=500][Space=2]
 Hostile or not, here I come![Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>That's what I thought.[Wait=500][Space=2]
-If they put me there in the first place, there is a reason, and I don't they did all of that just for fun.[Wait=500][Space=2]
-There is a meaning behind all of this mess I've been through and I want to know about it.[Wait=500][Space=2]
-And if they can free me in the process, it would be nice too.[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>I guess I'll be jumping right into it then![Wait=500][Space=2]
 I have no choice anyway. It's my only hope to get out of this island.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>Too bad you're not me and that I can make decisions on my own![Wait=500][Space=2]
-I've been on this island for hours and I know there is no way out outside.[Wait=500][Space=2]
-It's too late to change my mind.[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Yes, it is, and I totally understand that I'll be the only one responsible for the consequences of this decision.[Wait=500][Space=2]
 But I still count on you to help me here.[Wait=500][Space=2]</t>
   </si>
@@ -600,16 +439,8 @@
 But who was the one asking you these questions?[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>Yeah, as if you could pretend that![Wait=500][Space=2]
-Anyway, let's focus on the most important question : WHO WAS THAT?[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>I...[Wait=500] I heard everything.[Wait=500][Space=2]
 Were you sincere while answering these questions?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Are you serious...[Wait=500][Space=2]
-You know what forget it...[Wait=500] The most important think is who the fuck was this person asking you all this?[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>Fuck! The signal’s scram-[Color=Gray]*SHKRRRRRRRRR*[Color=White]...[Wait=500] There must be a way to-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]...[Wait=500] [Color=Gray]*Snap*[Color=White]...[Wait=500][Space=2]
@@ -658,80 +489,10 @@
 ...[Wait=500] What is that?[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>I'm chicken-hearted?[Wait=500] Oh yeah?[Wait=500][Space=2]
-Well, you know what?[Wait=500] I'll enter this museum without you begging me for it![Wait=500][Space=2]
-[Color=Gray]*Footsteps*[Color=White][Wait=500] [Color=Gray]*WHAM*[Color=White]...[Wait=500][Space=2]
-HEY![Wait=500] I JUST ENTERED YOUR MUSEUM BY KICKING THE DOOR! [Color=Gray]*Echoes*[Color=White]...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>See?[Wait=500] I can get cocky when I want![Wait=500] RIGHT?! [Color=Gray]*Echoes*[Color=White]...[Wait=500][Space=2]
-...[Wait=500] Yeah, no one's responding.[Wait=500] Not that I'm disappointed anyway![Wait=500][Space=2]
-It's way better to know that there is no one lurking at me ahah![Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>If I would listen to me, I would not enter this place because it freaks me out for some reason...[Wait=500][Space=2]
-But you're here! I've got nothing to be afraid of, so I'm heading inside![Wait=500][Space=2]
-[Color=Gray]*Footsteps*[Color=White][Wait=500] [Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Oh freak...[Wait=500] It means my instinct didn't betray me?[Wait=500][Space=2]
-Do you think it's here? Observing me from a corner?[Wait=500][Space=2]
-[Color=Gray]*Heavy brething*[Color=White]...[Wait=500] I think I'm going to throw up...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Phew...[Wait=500] That's true.[Wait=500][Space=2]
-I'm not in imminent danger...[Wait=500] I must focus on my escape and everything will be okay![Wait=500][Space=2]
-I needed to reassure myself before doing a bit of exploration, sorry.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Huh?[Wait=500] [Color=Gray]*Heavy breathing*[Color=White][Wait=500] I don't care about the art![Wait=500][Space=2]
-You know it's really not the time to be joking around, right?[Wait=500][Space=2]
-I'm diving into the unknown and you think it's funny?[Wait=500] That's really irritating![Wait=500][Space=2]
-I don't want to argue here, so let's go see what this museum has to offer.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Gray]*Footsteps*[Color=White]...[Wait=500] The paintings are all representation of a city![Wait=500][Space=2]
-Seems like the keeper of this museum really liked it.[Wait=500] I can see similar features between all of them.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Gray]*Footsteps*[Color=White]...[Wait=500] Oh wow! They look even more muscular from close![Wait=500][Space=2]
-These stony guys are fighting reeaaaal good![Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Gray]*Footsteps*[Color=White]...[Wait=500] It's a really good looking rock, with good looking inscriptions on it![Wait=500][Space=2]
-Too bad, I can't speak that language tho.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>I thought the same thing...[Wait=500] I'm not here to appreciate the beauty of hand-made art.[Wait=500][Space=2]
-I'm here to GET OUT OF THIS ISLAND![Wait=500] FUCK YOU, ART![Wait=500][Space=2]
-[Color=Gray]*CRACK*[Color=White][Wait=500] Shit, I didn't know kicking a statue could dislock it's leg-[Color=Gray]*RUMBLE*[Color=White]...[Wait=500] Huh?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>I don't know, but I'm too curious to not go and see what this damn door is all about![Wait=500][Space=2]
-[Color=Gray]*Footsteps*[Color=White]...[Wait=500] SHIT! It's locked![Wait=500][Space=2]
-There's a keypad attached to it.[Wait=500] And it's weird but...[Wait=500] there are letters here instead of numbers.[Wait=500][Space=2]
-Oh![Wait=500] And here you go, another post-it![Wait=500] I start to identify a leitmotiv in these puzzles...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>It say:[Wait=500][Space=2]
-[Color=Green]"IN CASE THE MADNESS MAKES YOU FORGET:[Wait=500][Space=2]
--FIRST LETTER = CITY NAME.[Wait=500][Space=2]
--SECOND LETTER = ARTIST NAME.[Wait=500][Space=2]
--THIRD LETTER = TRANSLATED IN ENGLISH.[Wait=500][Space=2]
-KEEP EVERYONE OUT AT ALL COST."[Color=White][Wait=500][Space=2]
-...[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>It's a flat piece of rock with engravings on it.[Wait=500][Space=2]
 It seems to be a dead language I don't know how to read.[Wait=500][Space=2]
 There is one word on here that's colored in red.[Wait=500][Space=2]
 It reads [Color=Green]"Effingo"[Color=White].[Wait=500] I hope I pronounced it properly.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>...[Wait=500] I'm shaking of fear, but I need to concentrate to click on the right button...[Wait=500][Space=2]
-[Color=Gray]*B[Beep=True]#eep*[Color=White]...[Wait=500][Space=2]
-Oh yes! it didn't explode or anything, so we may be on the right path![Wait=500][Space=2]
-The second letter was [Color=Green]"ARTIST NAME"[Color=White].[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>If I die because of this, I'll kill you, remember that...[Wait=500][Space=2]
@@ -751,13 +512,6 @@
 [Color=Gray]*Cough*[Color=White][Wait=500] Why is everything get-[Color=Gray]*Cough*[Color=White]...[Wait=500] getting blurry?[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>[Color=Gray]*Cough*[Color=White] [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
-I c...[Wait=500] [Color=Gray]*Cough*[Color=White][Wait=500] I can't breath![Wait=500][Space=2]
-[Color=Gray]*Cough*[Color=White][Wait=500] [Color=Gray]*COUGH*[Color=White] [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
-Arhh...[Wait=500][Space=2]
-...[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Please be right, please be right, please be right...[Wait=500][Space=2]
 [Color=Gray]*B[Beep=True]eep*[Color=White]...[Wait=500][Space=2]
 [Color=Gray]*CLICK*[Color=White][Wait=500] The door... is unlocked![Wait=500][Space=2]
@@ -765,45 +519,8 @@
 [Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>I'm down the stairs.[Wait=500] It see-[Color=Gray]*SHKRRRRRRRRRR*[Color=White].[Wait=500][Space=2]
-There's multiple corridor leading to-[Color=Gray]*SHKRRRRRRRRRR*[Color=White]...[Wait=500] I don't know which one is the right one![Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Hell-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]-ou hear me?[Wait=500][Space=2]
 Why did you stop spea-[Color=Gray]*SHKRRRRRRRRRRRR*[Color=White].[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Of course you don't...[Wait=500][Space=2]
-The more I realise the situation I'm in, the less I think all of this makes sense...[Wait=500][Space=2]
-Anyway, I'm inside a complex of whitish corridors, the-[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
-Wait...[Wait=500] Those footsteps weren't mine...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Gray]*Footsteps*[Color=White] It's getting closer![Wait=500][Space=2]
-[Color=Gray]*SLAM*[Color=White]...[Wait=500][Space=2]
-I locked myself inside a room...[Wait=500] I think I'm safe n-.[Wait=500][Space=2]
-[Color=Yellow]It's useless to hide you know?[Wait=500] I know where you are at all time[Color=White][Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Yellow]No matter what your friend says, it's just between me and you subject 835...[Color=White][Wait=500][Space=2]
-[Color=Yellow]You bypassed what I've prepared for you by entering the museum. It never happened before![Color=White][Wait=500][Space=2]
-W-Who are you calling subject 835?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Yellow]Subject 835?[Wait=500] That's you of course![Color=White][Wait=500][Space=2]
-[Color=Yellow]You're no more than a pale copy of the one you're calling on this phone right now.[Color=White][Wait=500][Space=2]
-W-Wait...[Wait=500] What?[Wait=500] A copy you say?[Wait=500][Space=2]
-[Color=Yellow]A clone, if you prefer this term.[Color=White][Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>No...[Wait=500] It's impossible![Wait=500] YOU'RE LYING![Wait=500][Space=2]
-[Color=Yellow]...I expected this kind of reaction.[Wait=500] Why do you think you and the original behind this call have the same voice?[Color=White][Wait=500][Space=2]
-[Color=Yellow]Didn't it strike you at first that he was the only contact on this phone?[Color=White][Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Yellow]I'm telling you the truth.[Wait=500] It might seem troubling but you have to accept that you're just a mere reproduction.[Color=White][Wait=500][Space=2]
-[Color=Yellow]But why would it matter?[Wait=500] You're now the perfect subject I was waiting for.[Color=White][Wait=500][Space=2]
-...[Wait=500] What do you mean by...[Wait=500] The perfect subject?[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>[Color=Yellow]Do you think I prepared all of this for fun?[Color=White][Wait=500][Space=2]
@@ -811,17 +528,6 @@
 ...[Wait=500] 832?[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>[Color=Yellow]Not all.[Wait=500] I just said that you were subject 835.[Wait=500] 3 are still alive to this day.[Color=White][Wait=500][Space=2]
-[Color=Yellow]One was not able to handle the virus. However he managed to take out his tracker and he's still roaming outside.[Color=White][Wait=500][Space=2]
-[Color=Yellow]He was responsible for the death of some clones because of his hostility.[Color=White][Wait=500][Space=2]
-[Color=Yellow]The other one was immune, but he managed to bypass my security and to free himself.[Color=White][Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Yellow]Oh?[Wait=500] He contacted you?[Wait=500] How curious, this must mean he's still on the island.[Color=White][Wait=500][Space=2]
-[Color=Magenta][Beep=True]DoN[Wait=500][Beep=True]'t tRu[Wait=500][Beep=True]st hIm[Wait=500][Beep=True].  aLl oF[Wait=500][Beep=True]  tHeSe dEa[Wait=500][Beep=True]tHs iS[Wait=500][Beep=True]  bEcAuSe[Wait=500][Beep=True]  oF hIm.[Color=White][Wait=500][Space=2]
-...[Wait=500] I can't believe all that...[Wait=500] Why am I here![Wait=500] TELL ME WHY DID YOU MADE ME![Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>SPEAK TO M-[Color=Gray]*SHKRRRRRRRR*[Color=White].[Wait=500][Space=2]
 I don-[Color=Gray]*SHKRRRRR*[Color=White]-ear you![Wait=500][Space=2]
 [Color=Magenta][Beep=True]He[Wait=500][Beep=True] cA[Wait=500][Beep=True] n’T[Wait=500][Beep=True]  He[Wait=500][Beep=True] aR[Wait=500][Beep=True] yO[Wait=500][Beep=True] u aN[Wait=500][Beep=True] yMo[Wait=500][Beep=True] re,[Wait=500][Beep=True]  bUt[Wait=500][Beep=True]  i[Wait=500][Beep=True] cA[Wait=500][Beep=True] n He[Wait=500][Beep=True] lP[Wait=500][Beep=True] hIm.[Color=White][Wait=500][Space=2]</t>
@@ -848,130 +554,18 @@
     <t>[Color=Magenta][Beep=True]I[Wait=500][Beep=True] f yOu[Wait=500][Beep=True]  wErE aT[Wait=500][Beep=True]  iTs[Wait=500][Beep=True]  pLaCe,[Wait=500][Beep=True]  wOuLd[Wait=500][Beep=True]  yOu[Wait=500][Beep=True]  hAvE[Wait=500][Beep=True]  tRuStEd[Wait=500][Beep=True]  tHe[Wait=500][Beep=True]  oNe[Wait=500][Beep=True]  bEhInD[Wait=500][Beep=True]  tHe[Wait=500][Beep=True]  pHoNe[Wait=500][Beep=True]  yOu[Wait=500][Beep=True]  fOuNd?[Color=White][Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>[Color=Magenta][Beep=True]Th[Wait=500][Beep=True] aT[Wait=500][Beep=True]  wI[Wait=500][Beep=True] lL dO[Wait=500][Beep=True]... Th[Wait=500][Beep=True] aNkS fO[Wait=500][Beep=True] r Y[Wait=500][Beep=True] oU r H[Wait=500][Beep=True] eLp.[Color=White][Wait=500][Space=2]
-...[Color=Gray]*SHKRRRR*[Color=White] Hello?[Wait=500 Hey?[Wait=500][Space=2]
-Can you hear me?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Yellow]I understand your confusion.[Wait=500] But the survival of humankind is at stake at this very moment.[Color=White][Wait=500][Space=2]
-[Color=Yellow]A virus is spreading, and it's undetectable.[Wait=500] I called it the Emotoxin.[Wait=500] No one believed me.[Color=White][Wait=500][Space=2]
-[Color=Yellow]It decuplates the instensity of our emotions, causing us to burst out of rage, euphoria or feel miserable.[Color=White][Wait=500][Space=2]
-...[Wait=500] And in what way could this cause the end of humankind?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Yellow]You should see how an infected acts.[Color=White][Wait=500][Space=2]
-[Color=Yellow]In our world filled with hate, it would cause people to kill each other over a small argument.[Color=White][Wait=500][Space=2]
-...[Wait=500] I'm not infected right?[Wait=500] So why would you do all that in the first place![Wait=500][Space=2]
-Why not use a lab rat instead of killing HUNDREDS OF HUMANS![Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Yellow]The Emotoxin only affects humans. So I preffered to base my search on clones instead of real humans.[Color=White][Wait=500][Space=2]
-[Color=Yellow]I chose to clone you because your DNA was highly compatible with cloning and resistent to the Emotoxin structure.[Color=White][Wait=500][Space=2]
-[Color=Yellow]All these puzzles were tests to see if you were affected by the toxin by playing with your emotions.[Color=White][Wait=500][Space=2]
-[Color=Yellow]I think it might be time to get out of this room now.[Wait=500] I need your blood.[Color=White][Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Y-Yes![Wait=500] I'M STAYING INSIDE YOU PSYCHOPATH![Wait=500][Space=2]
-I'M NOT GOING TO LET YOU SUCK MY BLOOD![Wait=500] I MAY BE A CLONE BUT I'M NOT BELIEVING ALL THIS SHIT![Wait=500][Space=2]
-[Color=Yellow]...[Wait=500] Hmmm...[Wait=500] Unfortunatly for you, I anticipated this kind of reaction.[Color=White][Wait=500][Space=2]
-[Color=Yellow]What are your last words?[Color=White][Wait=500][Space=2]
-Y-You're bluffing![Wait=500] I'm not going to fall for this eith-[Color=Gray]*PSHHHHHHHHHH*[Color=White]...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>...[Wait=500] OH SHIT![Wait=500] THERE'S GREEN GAS SPREADING IN THE ROOM![Wait=500][Space=2]
-[Color=Gray]*Door shake*[Color=White]...[Wait=500][Space=2]
-LET ME OUT, THIS FUCKER LOCKED THE DOOR![Wait=500][Space=2]
-[Color=Yellow]You made your own choices you and your friend.[Wait=500] Now you'll have to accept the consequences.[Color=White][Wait=500][Space=2]
-[Color=Gray]*Cough*[Color=White]... No...[Wait=500] [Color=Gray]*Cough*[Color=White] [Color=Gray]*Cough*[Color=White]...[Wait=500][Space=2]
-.[Wait=500].[Wait=500].[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>[Color=Gray]*B[Beep=True]eep*[Color=White]...[Wait=500] [Color=Gray]*B[Beep=True]eep*[Color=White]...[Wait=500] [Color=Gray]*B[Beep=True]eep*[Color=White]...[Wait=500][Space=2]
 [Color=Gray]{INCOMING CALL: UNKNOWN}[Color=White]...[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>N-NO![Wait=500] I WON'T FOLLOW HIM![Wait=500][Space=2]
-I DON'T TRUST YOU ANYMORE![Wait=500] You were plotting with him since the beggining right?[Wait=500][Space=2]
-[Color=Gray]*SLAM*[Color=White] OUCH![Wait=500] I'M GETTING OUT OF HERE![Wait=500][Space=2]
-[Color=Gray]*Fast footsteps*[Color=White]...[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>Everything makes sense for me now![Wait=500] You were planning all of this with him! [Color=Gray]*Fast footsteps*[Color=White]...[Wait=500][Space=2]
 Huff...[Wait=500] Who tells me you're not on this island too, monitoring me in one of these rooms?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>LIAR![Wait=500][Space=2]
-You could be behind THIS DOOR [Color=Gray]*SLAM*[Color=White]...[Wait=500][Space=2]
-THIS DOOR [Color=Gray]*SLAM*[Color=White]...[Wait=500][Space=2]
-...[Wait=500] Ah AH! Just as I thought, a monitoring room![Wait=500][Space=2]
-You were here before huh?[Wait=500] Planning for the next puzzle and acting as if you were discovering it with me.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>You're the crazy one here, cloning yourself and watch you suffer with this mad scientist![Wait=500][Space=2]
-...[Wait=500] Oh![Wait=500] Look![Wait=500] How unfortunate for you![Wait=500][Space=2]
-"This button should only be used in case that the Emotoxin breaches out.[Wait=500][Space=2]
-The explosion will eradicate all living organism in a 5 kilometers."[Wait=500][Space=2]
-...[Wait=500] You really put a self-destruct button here?[Wait=500] Too bad, because I'm going to press it.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>AND I WILL ALSO KILL YOU AND YOUR SCIENTIST FRIEND![Wait=500][Space=2]
-I will end this whole madness![Wait=500] Hundreds of different versions of you were killed.[Wait=500] THEY HAD FEELINGS YOU KNOW?![Wait=500][Space=2]
-I'm willing to sacrifice, as a revenge for all the ones that suffered before me.[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>Have a good death, original.[Wait=500][Space=2]
 [Color=Gray]*Click*[Color=White]...[Wait=500][Space=2]
 .[Wait=500].[Wait=500].[Wait=500][Space=2]
 [Color=Gray]*BOOOOOOOOOMMMMMMM*[Color=White]...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>...[Wait=500] Is it really for the survival of humanity?[Wait=500] It's not a trick so that I get out and you can shoot me easily?[Wait=500][Space=2]
-[Color=Yellow]Absolutely not.[Wait=500] I care for my research, and I wouldn't waste any of my bullets or any of your blood.[Color=White][Wait=500][Space=2]
-...[Wait=500] [Color=Gray]*Door opening*[Color=White]...[Wait=500] [Color=Yellow]So you opened.[Color=White][Wait=500][Space=2]
-I don't know what you mean by needing my blood but I assume this will not be pleasurable?[Wait=500][Space=2]
-[Color=Yellow]You guessed it. But I will do what's possible to keep you alive after that?[Color=White][Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Yellow]I'm a scientist, not a social expert.[Wait=500] Now, original,  we have to end the call here.[Wait=500] I have to borrow this clone.[Color=White][Wait=500][Space=2]
-W-Wait... I have a question.[Wait=500] Why did you make us contact each other?[Wait=500][Space=2]
-[Color=Yellow]I needed a full panel of your emotions right when I knew that you were the right one.[Color=White][Wait=500][Space=2]
-[Color=Yellow]There was no better options than using yourself as to stimulate every aspect of your personnality.[Color=White][Wait=500][Space=2]
-[Color=Yellow]Talking to yourself shows how the human behaviour is not absolute for a single person.[Color=White][Wait=500][Space=2]
-[Color=Yellow]The gap between what we think we'd do and what we actually do is indeterminatable.[Color=White][Wait=500][Space=2]
-[Color=Yellow]By calling the original, you could explore every aspect of yourself...[Color=White][Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Yellow]Good.[Wait=500] Now, original, you'll excuse us but we have to end the call here.[Wait=500] I have to borrow this clone.[Color=White][Wait=500][Space=2]
-W-Wait... I have a question.[Wait=500] Why did you make us contact each other?[Wait=500][Space=2]
-[Color=Yellow]I needed a full panel of your emotions right when I knew that you were the right one.[Color=White][Wait=500][Space=2]
-[Color=Yellow]There was no better options than using yourself as to stimulate every aspect of your personnality.[Color=White][Wait=500][Space=2]
-[Color=Yellow]Talking to yourself shows how the human behaviour is not absolute for a single person.[Color=White][Wait=500][Space=2]
-[Color=Yellow]The gap between what we think we'd do and what we actually do is indeterminatable.[Color=White][Wait=500][Space=2]
-[Color=Yellow]By calling the original, you could explore every aspect of yourself...[Color=White][Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Yellow]Confusing, I know.[Wait=500] Even if I vulgarise the terms, it's still a concept most won't understand.[Color=White][Wait=500][Space=2]
-...[Wait=500][Space=2]
-One more thing.[Wait=500] Can I talk one last time with the original?[Wait=500][Space=2]
-[Color=Yellow]Go on.[Wait=500] I've waited years for you to exist, so I can wait one more minute.[Color=White][Wait=500][Space=2]
-...[Wait=500] Hey...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>You bet it was![Wait=500] That's unfortunate that we have to end on this save the humanity tone...[Wait=500][Space=2]
-But I guess we can't do anything about it.[Wait=500][Space=2]
-The world chose you to be immune.[Wait=500] And by you, that includes me...[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Ahah![Wait=500] I guess you're right![Wait=500][Space=2]
-...[Wait=500] Thank you for staying with me...[Wait=500] I know I was just a random call of a stranger at the beginning but...[Wait=500][Space=2]
-But I hope I'll be able to call you again one day.[Wait=500] We'll be able to eat something at your favorite restaurant![Wait=500][Space=2]
-I know which one it is since I've got the same memories than you eheh![Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Ahahah![Wait=500] That's tru-.[Wait=500][Space=2]
-[Color=Yellow]We have to go.[Color=White][Wait=500][Space=2]
-O-Oh...[Wait=500] Well, I guess it's a goodbye.[Wait=500][Space=2]
-I really hope to see you again.[Wait=500] Until now, believe in yourself.[Wait=500] I know we're great people.[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>...[Wait=500][Space=2]
@@ -988,23 +582,10 @@
 [Color=Red]BAD ENDING.[Color=White][Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>...[Wait=500][Space=2]
-[Color=Red]--SIGNAL LOST--[Color=White][Wait=500][Space=2]
-[Color=Red]{YOU FAIL TO FIND THE RIGHT PASSWORD. MAYBE IF YOU'D TRIED HARDER?}[Color=White][Wait=500][Space=2]
-[Color=Red]BAD ENDING.[Color=White][Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>[Color=Gray]*Static*[Color=White]...[Wait=500][Space=2]
 .[Wait=500].[Wait=500].[Wait=500][Space=2]
 [Color=Red]--SIGNAL LOST--[Color=White][Wait=500][Space=2]
 [Color=Red]{NO ONE ANSWERED. NO ONE EVER WILL?}[Color=White][Wait=500][Space=2]
-[Color=Red]BAD ENDING.[Color=White][Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Gray]*Static*[Color=White]...[Wait=500][Space=2]
-.[Wait=500].[Wait=500].[Wait=500][Space=2]
-[Color=Red]--SIGNAL LOST--[Color=White][Wait=500][Space=2]
-[Color=Red]{YOU FAIL TO FIND THE RIGHT PASSWORD. MAYBE IF YOU'D TRIED HARDER?}[Color=White][Wait=500][Space=2]
 [Color=Red]BAD ENDING.[Color=White][Wait=500][Space=2]</t>
   </si>
   <si>
@@ -1019,16 +600,6 @@
     <t>[Choice1=[NextScene=2][Content=How much time will it take to get there?]]</t>
   </si>
   <si>
-    <t>[Color=Gray]*SHKRRRRRR*[Color=White]-MY GOD! I’ve been stuck here-[Color=Gray]*SHKRRRRRRRRRRR*[Color=white]-for days. Tt feels so good to hear someone’s voice...[Wait=500][Space=2]
-[Color=Gray]*SHKRRRRRRRRRRRRRRRR*[Color=White]-Any idea what’s happening? Who are y-[Color=Gray]*SHKRRRRRRRRRRRRRRRR*[Color=White]-I, and why I am here?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Gray]*Click*[Color=White]...[Wait=500][Space=2]
-[Color=Gray]*SHKRRRRRRRRR*[Color=White]...H-Hello? Is someone the-[Color=Gray]*SHKRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
-How does this thing wor-[Color=Gray]*SHKRRRRRRRRRR*[Color=White]...[Wait=500] Can you hear m-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
-Hello?[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>I’m-[Color=Gray]*SHKRRRRRRRRR*[Color=White]. I don’t know how-[Color=Gray]*SHKRRRRRRRRR*[Color=White]-I can't get out...[Wait=500][Space=2]
 And you-[Color=Gray]*SHKRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
 Are-[Color=Gray]*SHKRRRRRRRR*[Color=White]-still there?[Wait=500][Space=2]</t>
@@ -1042,11 +613,6 @@
 I-I’m all alone on this weird island. I’ve been searching for someone for hours now.[Wait=500][Space=2]
 All I’ve managed to find are more ruins.[Wait=500][Space=2]
 It's like an abandoned city.[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Can’t even tell! I just found this old-ass flip phone on a shelf.[Wait=500][Space=2]
-It started a call the moment I opened it![Wait=500][Space=2]
-There's nothing else on that piece of junk, no contacts, no internet access, just this call number.[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>[Choice1=[NextScene=12][Content=Are you in any danger?]]
@@ -1079,13 +645,6 @@
 Listen, it seems like you’re the only one I can rely on right now.[Wait=500][Space=2]
 You’re literally the first person I’ve talked to in the past few hours, or even days![Wait=500][Space=2]
 You’re my only way to communicate with the outside world, it’s just a matter of keeping my sanity at this point![Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>PLEASE DON’T HANG UP! I just need someone to talk to![Wait=500][Space=2]
-I have no idea if either of us will even be able to call again if you hang up![Wait=500][Space=2]
-Wh-[Wait=500] whatever is happening to me is beyond anything they could believe anyway![Wait=500][Space=2]
-...[Wait=500][Space=2]
-[Color=Magenta][Beep=True]It[Wait=500][Beep=True] wO[Wait=500][Beep=True] uLd[Wait=500][Beep=True] bE uS[Wait=500][Beep=True] eLLeSs.[Wait=500][Beep=True]  Ke[Wait=500][Beep=True] p tHe[Wait=500][Beep=True] CaLL[Wait=500][Beep=True] gO[Wait=500][Beep=True] iNg.[Color=White][Wait=500][Space=2]</t>
   </si>
   <si>
     <t>PLEA-[Color=Gray]*B[Beep=True]eep*[Color=White]...[Wait=500][Space=2]
@@ -1309,34 +868,14 @@
 Anyway, you might want to search for that on the internet, it's a 4-digit password.[Wait=500] I'll try to log in.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>[Choice1=[NextScene=3][Content=Small?]]
-[Choice2=[NextScene=4][Content=Well preserved?]]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=13][Content=Why are you doubting all of a sudden?]]
 [Choice2=[NextScene=14][NextSceneNoTrust=13][TrustNeed=50][Content=Well, you might as well go and see inside to be sure!]]</t>
   </si>
   <si>
-    <t>[Choice1=[NextScene=5][TrustAdd=25][Content=Nah. Why would someone want to clean an old museum anyway? It's a coincidence.]]
-[Choice2=[NextScene=6][Content=I guess there is, why would it be cleaner than the other building otherwise?]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=6][Content=You're afraid of seeing someone now?]]
-[Choice2=[NextScene=7][TrustAdd=-25][Content=Well, don't enter it then.]]
-[Choice3=[NextScene=8][Content=Sorry to announce that, but it doesn't seem that you have the choice...]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=8][TrustAdd=25][Content=Everything's gonna be fine as long as we collaborate.]]
-[Choice2=[NextScene=9][TrustAdd=-25][Content=I knew it! You're chicken-hearted!]]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=8][TrustAdd=25][Content=You're not in danger as long as I'm with you!]]
 [Choice2=[NextScene=9][Content=I knew you were chicken-hearted!]]</t>
   </si>
   <si>
-    <t>[Choice1=[NextScene=15][Content=Is there something weird in here?]]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=10][TrustAdd=-25][Content=Shhhh!! What if there's really someone here?]]
 [Choice2=[NextScene=11][Content=That's more like it!]]</t>
   </si>
@@ -1344,65 +883,7 @@
     <t>[Choice1=[NextScene=15][Content=What makes you feel like that?]]</t>
   </si>
   <si>
-    <t>[Choice1=[NextScene=12][TrustAdd=25][Content=Well... I am]]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=15][Content=What about it?]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=6][Content=You're afraid of seeing someone now?]]
-[Choice2=[NextScene=7][TrustAdd=-25][Content=Well, don't enter it then.]]
-[Choice3=[NextScene=8][Content=Sorry to announce that, but it doesn't seem that you have the choice...]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=15][Content=So? What's inside?]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=16][Content=That's weird...]]
-[Choice2=[NextScene=17][TrustAdd=-25][Content=That's so cool!]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=18][TrustAdd=-25][Content=You're becoming paranoïd?]]
-[Choice2=[NextScene=19][Content=Someone's living here?]]
-[Choice3=[NextScene=20][TrustAdd=25][Content=That we have a new mystery to resolve!]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=18][TrustAdd=-25][Content=You're definitly becoming paranoïd.]]
-[Choice2=[NextScene=19][Content=Is... someone living here?]]
-[Choice3=[NextScene=20][TrustAdd=25][Content=Seems that we'll have to solve this mystery together!]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=21][TrustAdd=-25][Content=I think I would be braver than you!]]
-[Choice2=[NextScene=22][TrustAdd=25][Content=I think I'd manage things like you.]]
-[Choice3=[NextScene=23][Content=I'd be... more fearful than you!]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=24][TrustAdd=25][Content=Calm Down. That doesn't justify any panic.]]
-[Choice2=[NextScene=25][TrustAdd=-25][Content=Don't throw up on the art please.]]
-[Choice3=[NextScene=26][TrustAdd=-25][Content=I was joking around! There's surely not anyone here.]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=27][Content=What is around you again?]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=28][Content=Go and see the paintings.]]
-[Choice2=[NextScene=29][Content=Go and see the sculpture.]]
-[Choice3=[NextScene=30][Content=Go and see the inscriptions on the rock.]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=31][Content=Is there something else than art here?]]
-[Choice2=[NextScene=39][Content=Can you describe it more precisely?]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=31][Content=Is there something else than art here?]]
-[Choice2=[NextScene=40][Content=Can you describe it more precisely?]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=31][Content=Is there something else than art here?]]
-[Choice2=[NextScene=41][Content=Can you describe it more precisely?]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=32][Content=What's going on?]]</t>
   </si>
   <si>
     <t>[Choice1=[NextScene=33][Content=It must be a secret escape!]]
@@ -1479,19 +960,11 @@
 [Choice3=[Quit=True][Content=Quit.]]</t>
   </si>
   <si>
-    <t>[Choice1=[NextScene=53][Content=What are you expecting to find here?]]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=54][Content=What if you don't find any fuse?]]
 [Choice2=[NextScene=58][Content=What if there was someone down there?]]
 [Choice3=[NextScene=61][Content=What if it's a trap?]]</t>
   </si>
   <si>
-    <t>[Choice1=[NextScene=55][TrustAdd=25][Content=Of course! I will be with you until the end.]]
-[Choice2=[NextScene=56][TrustAdd=-25][Content=Uhm, I have more alluring stuff to do.]]
-[Choice3=[NextScene=57][TrustAdd=25][Content=Sorry but I don't feel confortable with hearing someone slowly dying on phone...]]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=64][Content=I was just being honest! You're down the stairs?]]</t>
   </si>
   <si>
@@ -1501,17 +974,6 @@
     <t>[Choice1=[NextScene=64][Content=Funny one. You're down the stairs?]]</t>
   </si>
   <si>
-    <t>[Choice1=[NextScene=59][TrustAdd=-25][Content=But they'll be hostile!]]
-[Choice2=[NextScene=60][Content=Maybe we can deal so they free you.]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=64][Content=Where ar you now?]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=62][TrustAdd=-25][Content=I would go back and search for another way out if I were you.]]
-[Choice2=[NextScene=63][Content=Do whatever you want, it's your responsability.]]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=64][Content=So you're getting down there?]]</t>
   </si>
   <si>
@@ -1519,11 +981,6 @@
   </si>
   <si>
     <t>[Choice1=[NextScene=65][Content=Shit! The signal's getting weaker again!]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Choice1=[NextScene=66][Content=Can you hear me?]]
-[Choice2=[NextScene=66][Content=I'm still here!]]
-</t>
   </si>
   <si>
     <t>[Choice1=[NextScene=67][Content=Who is this?]]</t>
@@ -1611,9 +1068,6 @@
     <t>[Choice1=[NextScene=91][Content=What is this noise?]]</t>
   </si>
   <si>
-    <t>[Choice1=[NextScene=92][Content=DONT GIVE UP!]]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=94][Content=You're getting everything wrong!]]
 [Choice2=[NextScene=95][Content=Why are you acting like this?!]]</t>
   </si>
@@ -1651,11 +1105,564 @@
 [Choice2=[NextScene=105][Content=It's you that will save the world in the end, not me.]]</t>
   </si>
   <si>
-    <t>[Choice1=[NextScene=106][Content=We'll go and see a movie too! Since your favorites one are also mine.]]
+    <t>[Choice1=[NextScene=107][Content=See you later.]]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*Click*[Color=White]...[Wait=500][Space=2]
+[Color=Gray]*SHKRRRRRRRRR*[Color=White]...H-Hello? Is someone there-[Color=Gray]*SHKRRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
+How does this thing wor-[Color=Gray]*SHKRRRRRRRRRR*[Color=White]...[Wait=500] Can you hear m-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]...[Wait=500][Space=2]
+Hello?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*SHKRRRRRR*[Color=White]-MY GOD! I’ve been stuck here-[Color=Gray]*SHKRRRRRRRRRRR*[Color=White]-for days. It feels so good to hear someone’s voice...[Wait=500][Space=2]
+[Color=Gray]*SHKRRRRRRRRRRRRRRRR*[Color=White]-Any idea what’s happening? Who are y-[Color=Gray]*SHKRRRRRRRRRRRRRRRR*[Color=White]-I, and why am I here?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Can’t even tell! I just found this old flip phone on a shelf.[Wait=500][Space=2]
+It started a call the moment I opened it![Wait=500][Space=2]
+There's nothing else on that piece of junk, no contacts, no internet access, just this call number.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>PLEASE DON’T HANG UP! I just need someone to talk to![Wait=500][Space=2]
+I have no idea if either of us will even be able to call again if you hang up![Wait=500][Space=2]
+Wh-[Wait=500] whatever is happening to me is beyond anything they could believe anyway![Wait=500][Space=2]
+...[Wait=500][Space=2]
+[Color=Magenta][Beep=True]It[Wait=500][Beep=True] wO[Wait=500][Beep=True] uLd[Wait=500][Beep=True] bE uS[Wait=500][Beep=True] eLLeSs.[Wait=500][Beep=True] Ke[Wait=500][Beep=True] p tHe[Wait=500][Beep=True] CaLL[Wait=500][Beep=True] gO[Wait=500][Beep=True] iNg.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Going to the museum?[Wait=500] I can work with that.[Wait=500][Space=2]
+This whole trapdoor thing is suspicious anyway.[Wait=500] It might be better to explore this place before doing anything stupid.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>It's not that far away. I think I can even see it from here![Wait=500] I'll take you back in a second once I'm there![Wait=500][Space=2]
+.[Wait=500].[Wait=500].[Wait=500][Space=2]
+.[Wait=500].[Wait=500].[Wait=500][Space=2]
+Okay![Wait=500] I'm in front of it.[Wait=500] It's smaller than I thought, and it looks really well-preserved![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>That's weird, right?[Wait=500][Space=2]
+All the other places here are just empty buildings withered by time.[Wait=500][Space=2]
+It's strange that a useless building is still standing unharmed.[Wait=500][Space=2]
+...[Wait=500] Does that mean someone's still here to make sure this museum stays clean?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I'm sure you're right...[Wait=500] But it still feels odd.[Wait=500][Space=2]
+Great.[Wait=500] Now I don't even feel like entering this place.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I guess I am...[Wait=500] The fact that everything seems designed to make me explore this place is...[Wait=500][Space=2]
+Yes, I'm scared...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I FEEL like not entering, but I have no choice and you know it well![Wait=500][Space=2]
+I-...[Wait=500] I could do that, but nothing comes to mind that could help me escape.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I'm chicken-hearted?[Wait=500] Oh yeah?[Wait=500][Space=2]
+Well, you know what?[Wait=500] I'll enter this museum without you begging me to![Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White][Wait=500] [Color=Gray]*WHAM!*[Color=White]...[Wait=500][Space=2]
+HEY![Wait=500] I JUST ENTERED YOUR MUSEUM BY KICKING THE DOOR! [Color=Gray]*Echoes*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>What did I hear?[Wait=500] Is someone getting scared all of a sudden?[Wait=500] That’ll teach you![Wait=500][Space=2]
+But there doesn’t seem to be anyone here anyway.[Wait=500][Space=2]
+Looks like we both worried for nothing.[Wait=500][Space=2]
+...[Wait=500] But there’s still something off-putting here.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>See?[Wait=500] I can get cocky when I want![Wait=500] RIGHT?! [Color=Gray]*Echoes*[Color=White]...[Wait=500][Space=2]
+...[Wait=500] Yeah, no one’s responding.[Wait=500] Not that I’m disappointed anyway![Wait=500][Space=2]
+It’s way better to know there’s no one lurking around, ahah![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>That’s fair, but you seem like a good guy.[Wait=500][Space=2]
+I’m not going to be scared by a voice coming from an old flip phone![Wait=500][Space=2]
+But let’s focus on this museum now.[Wait=500] Something’s off.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500] I don’t think going inside the only building that looks inhabited is a good idea.[Wait=500][Space=2]
+I don’t want to end up face-to-face with someone hostile.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>If I were to listen to myself, I wouldn’t enter this place because it freaks me out for some reason...[Wait=500][Space=2]
+But you’re here! I’ve got nothing to be afraid of, so I’m heading inside![Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White][Wait=500] [Color=Gray]*Door squeak*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>The inside of this museum truly feels abnormal...[Wait=500][Space=2]
+Everything’s clean. There’s not a single bit of dust here![Wait=500][Space=2]
+All these paintings are perfectly displayed,[Wait=500] the sculptures are brightly polished...[Wait=500][Space=2]
+There are even historical relics preserved under glass domes![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>It definitely is![Wait=500] How can this museum be this clean?[Wait=500][Space=2]
+Considering it’s the first place on this island that doesn’t look post-apocalyptic...[Wait=500][Space=2]
+It surely means that...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500] No, it isn’t![Wait=500][Space=2]
+It’s unsettling...[Wait=500] Every place I’ve been to on this island has been nothing but ruins, and now this![Wait=500][Space=2]
+It most definitely means that this place is special somehow...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500] What?[Wait=500] Wouldn’t you be paranoid after going through what I’m living?[Wait=500][Space=2]
+I’d like us to switch places and see how you’d manage all this...[Wait=500][Space=2]
+How would you like that idea?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Oh freak...[Wait=500] So my instinct didn’t betray me?[Wait=500][Space=2]
+Do you think it’s here? Watching me from a corner?[Wait=500][Space=2]
+[Color=Gray]*Heavy breathing*[Color=White]...[Wait=500] I think I’m going to throw up...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500] I didn’t expect that kind of answer, but it feels weirdly refreshing![Wait=500][Space=2]
+It’s nice having someone who can de-dramatize the whole situation.[Wait=500][Space=2]
+Let’s go and solve this mystery then! Where should I go?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>That's a bold thing to say![Wait=500][Space=2]
+You really are a daredevil, huh?[Wait=500][Space=2]
+Well, I'm not, and you'll have to bear with it.[Wait=500][Space=2]
+To refocus on what's important, I think exploring this room might be helpful.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>You see?[Wait=500] I guess we're not so different after all![Wait=500][Space=2]
+Now, this philosophical question is interesting, but it won't help me escape from here, so let's explore this place![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Ah![Wait=500] You act all confident, but you couldn’t handle a quarter of what I’m going through![Wait=500][Space=2]
+...[Wait=500] I’m the one making fun of you, but in the end, I’m still the one stuck on this island...[Wait=500] Ironic.[Wait=500][Space=2]
+It might be the right time to come back to the main question: what is this place?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Phew...[Wait=500] That’s true.[Wait=500][Space=2]
+I’m not in imminent danger...[Wait=500] I just need to focus on my escape and everything will be okay![Wait=500][Space=2]
+I needed to reassure myself before doing a bit of exploration, sorry.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Huh?[Wait=500] [Color=Gray]*Heavy breathing*[Color=White][Wait=500] I don’t care about the art![Wait=500][Space=2]
+You know it’s really not the time to be joking around, right?[Wait=500][Space=2]
+I’m diving into the unknown and you think it’s funny?[Wait=500] That’s really irritating![Wait=500][Space=2]
+I don’t want to argue here, so let’s go see what this museum has to offer.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Well, I hope you’re not a comedian![Wait=500][Space=2]
+You know it’s really not the time to be joking around, right?[Wait=500][Space=2]
+I’m diving into the unknown and you think it’s funny?[Wait=500] That’s really irritating![Wait=500][Space=2]
+I don’t want to argue here, so let’s go see what this museum has to offer.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>There are paintings on the wall, from the Impressionist era, it seems.[Wait=500][Space=2]
+There are also all these sculptures of muscular men.[Wait=500] The Greek, heterocurious kind of sculpture, you know.[Wait=500][Space=2]
+And there are these rock plates with strange language engraved on them.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*Footsteps*[Color=White]...[Wait=500] The paintings are all representations of a city![Wait=500][Space=2]
+Seems like the keeper of this museum really liked it.[Wait=500] I can see similar features between all of them.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*Footsteps*[Color=White]...[Wait=500] Oh wow! They look even more muscular up close![Wait=500][Space=2]
+These stone guys are fighting reaaally hard![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*Footsteps*[Color=White]...[Wait=500] It’s a really good-looking rock, with good-looking inscriptions on it![Wait=500][Space=2]
+Too bad I can’t speak that language though.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I thought the same thing...[Wait=500] I’m not here to appreciate the beauty of handmade art.[Wait=500][Space=2]
+I’m here to GET OFF THIS ISLAND![Wait=500] FUCK YOU, ART![Wait=500][Space=2]
+[Color=Gray]*CRACK*[Color=White][Wait=500] Shit, I didn’t know kicking a statue could dislocate its leg—[Color=Gray]*RUMBLE*[Color=White]...[Wait=500] Huh?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I-I don’t know, the ground shook for a second...[Wait=500][Space=2]
+Wait...[Wait=500] What’s tha-...[Wait=500][Space=2]
+...Did a motherfucking door just appear at the back of the museum?![Wait=500][Space=2]
+Did I really activate a mechanism at random because of my rage?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I don’t know, but I’m too curious not to see what this damn door is all about![Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500] SHIT! It’s locked![Wait=500][Space=2]
+There’s a keypad attached to it.[Wait=500] And weirdly enough...[Wait=500] there are letters instead of numbers.[Wait=500][Space=2]
+Oh![Wait=500] And here we go, another post-it![Wait=500] I’m starting to see a pattern in these puzzles...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>It says:[Wait=500][Space=2]
+[Color=Green]"IN CASE THE MADNESS MAKES YOU FORGET:[Wait=500][Space=2]
+-FIRST LETTER = CITY NAME.[Wait=500][Space=2]
+-SECOND LETTER = ARTIST NAME.[Wait=500][Space=2]
+-THIRD LETTER = TRANSLATED IN ENGLISH.[Wait=500][Space=2]
+KEEP EVERYONE OUT AT ALL COSTS."[Color=White][Wait=500][Space=2]
+...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>There are paintings on the wall, from the Impressionist era, it seems.[Wait=500][Space=2]
+There are also all these sculptures of muscular men.[Wait=500] The Greek, heterocurious kind of sculpture, you know.[Wait=500][Space=2]
+There are also these rock plates with strange language engraved on them.[Wait=500][Space=2]
+And obviously, this weird door with that letter keypad and the note.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>It’s multiple paintings depicting the same city, it seems![Wait=500][Space=2]
+I can tell because of the same monument present in every one of them.[Wait=500][Space=2]
+It’s a huge white pillar with a golden urn of fire on top, or something like that.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>It’s a white statue of two men fighting.[Wait=500][Space=2]
+Well... I said two men, but not really.[Wait=500] One is a centaur, if I’m not mistaken.[Wait=500][Space=2]
+The human one is on top of him with a huge stick, ready to strike the centaur.[Wait=500][Space=2]
+That’s a cool-looking statue![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>It's multiple paintings picturing the same city, it seems![Wait=500][Space=2]
+I can tell that because of the same looking monument on every one of them.[Wait=500][Space=2]
+It's a huge white pillar with a golden urn of fire at the top, or something like that.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>It's a white statue of two men fighting.[Wait=500][Space=2]
+Well, I said two men, but not really.[Wait=500] One is a centaur if I'm not mistaken.[Wait=500][Space=2]
+The human one is on top of him with a huge stick, ready to strike the centaur.[Wait=500][Space=2]
+That's a cool-looking statue![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Are you sure?[Wait=500] I don't know what could happen if I type the wrong code, but I don't want to find out.[Wait=500][Space=2]
+You're confident?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500] I'm shaking with fear, but I need to concentrate to click on the right button...[Wait=500][Space=2]
+[Color=Gray]*B[Beep=True]#eep*[Color=White]...[Wait=500][Space=2]
+Oh yes! It didn't explode or anything, so we may be on the right path![Wait=500][Space=2]
+The second letter was [Color=Green]"ARTIST NAME"[Color=White].[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*Cough*[Color=White] [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
+I c...[Wait=500] [Color=Gray]*Cough*[Color=White][Wait=500] I can't breathe![Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White] [Color=Gray]*COUGH*[Color=White] [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
+Arhh...[Wait=500][Space=2]
+...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500][Space=2]
+[Color=Red]--SIGNAL LOST--[Color=White][Wait=500][Space=2]
+[Color=Red]{YOU FAILED TO FIND THE RIGHT PASSWORD. MAYBE IF YOU'D TRIED HARDER?}[Color=White][Wait=500][Space=2]
+[Color=Red]BAD ENDING.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>For now, all I see are stairs going deep down...[Wait=500][Space=2]
+But I hope that I'll find this fuse to activate the trapdoor outside.[Wait=500][Space=2]
+Or at least answers for why I'm here.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*Static*[Color=White]...[Wait=500][Space=2]
+.[Wait=500].[Wait=500].[Wait=500][Space=2]
+[Color=Red]--SIGNAL LOST--[Color=White][Wait=500][Space=2]
+[Color=Red]{YOU FAILED TO FIND THE RIGHT PASSWORD. MAYBE IF YOU'D TRIED HARDER?}[Color=White][Wait=500][Space=2]
+[Color=Red]BAD ENDING.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>That's not reassuring to say, pal...[Wait=500][Space=2]
+What if there's no fuse?[Wait=500] Guess I'll die slowly, starving, while you're here listening to my agony.[Wait=500][Space=2]
+Would you be here to support me in my final moments?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Ahah![Wait=500] That was supposed to be a joke![Wait=500][Space=2]
+I admit that I wouldn't be able to handle that anyway.[Wait=500][Space=2]
+But if you're willing to hear me die, I guess that's okay![Wait=500] If that's not because of a twisted fantasy of yours...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Oh.[Wait=500] Uhm...[Wait=500][Space=2]
+Of course you have a life. I don't want to disturb you with my boring imminent death...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Ahah![Wait=500] Of course you're not![Wait=500] That was a joke![Wait=500][Space=2]
+Don't worry about it, if I ever find myself in this kind of situation, I wouldn't want you to suffer it too.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500] If we put together the door system and the tidiness of this museum compared to the other buildings...[Wait=500][Space=2]
+Yes, I think I'm about to meet the ones responsible for all my troubles.[Wait=500][Space=2]
+I don't know what their project is, but I'm sure I'll soon find out if I speak directly to them.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>That's what I thought.[Wait=500][Space=2]
+If they put me here in the first place, there’s a reason, and I don’t think they did all that just for fun.[Wait=500][Space=2]
+There must be meaning behind all this mess I've been through, and I want to know about it.[Wait=500][Space=2]
+And if they can free me in the process, that would be nice too.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Too bad you're not me and that I can make decisions on my own![Wait=500][Space=2]
+I've been on this island for hours, and I know there is no way out outside.[Wait=500][Space=2]
+It's too late to change my mind.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I'm down the stairs.[Wait=500] It see-[Color=Gray]*SHKRRRRRRRRRR*[Color=White].[Wait=500][Space=2]
+There are multiple corridors leading to-[Color=Gray]*SHKRRRRRRRRRR*[Color=White]...[Wait=500] I don't know which one is the right one![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Magenta][Beep=True]Th[Wait=500][Beep=True] aT[Wait=500][Beep=True] wI[Wait=500][Beep=True] lL dO[Wait=500][Beep=True]... Th[Wait=500][Beep=True] aNkS fO[Wait=500][Beep=True] r Y[Wait=500][Beep=True] oU r H[Wait=500][Beep=True] eLp.[Color=White][Wait=500][Space=2]
+...[Color=Gray]*SHKRRRR*[Color=White] Hello?[Wait=500] Hey?[Wait=500][Space=2]
+Can you hear me?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Yeah, as if you could pretend that![Wait=500][Space=2]
+Anyway, let's focus on the most important question: WHO WAS THAT?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Are you serious...[Wait=500][Space=2]
+You know what? Forget it...[Wait=500] The most important thing is who the hell was this person asking you all this?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Of course you don't...[Wait=500][Space=2]
+The more I realize the situation I'm in, the less I think all of this makes sense...[Wait=500][Space=2]
+Anyway, I'm inside a complex of whitish corridors, the-[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
+Wait...[Wait=500] Those footsteps weren't mine...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*Footsteps*[Color=White] It's getting closer![Wait=500][Space=2]
+[Color=Gray]*SLAM*[Color=White]...[Wait=500][Space=2]
+I locked myself inside a room...[Wait=500] I think I'm safe n-.[Wait=500][Space=2]
+[Color=Yellow]It's useless to hide, you know?[Wait=500] I know where you are at all times.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Yellow]No matter what your friend says, it's just between me and you, subject 835...[Color=White][Wait=500][Space=2]
+[Color=Yellow]You bypassed what I've prepared for you by entering the museum. It never happened before![Color=White][Wait=500][Space=2]
+W-Who are you calling subject 835?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Yellow]Subject 835?[Wait=500] That's you, of course![Color=White][Wait=500][Space=2]
+[Color=Yellow]You're no more than a pale copy of the one you're calling on this phone right now.[Color=White][Wait=500][Space=2]
+W-Wait...[Wait=500] What?[Wait=500] A copy, you say?[Wait=500][Space=2]
+[Color=Yellow]A clone, if you prefer this term.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>No...[Wait=500] It's impossible![Wait=500] YOU'RE LYING![Wait=500][Space=2]
+[Color=Yellow]...I expected this kind of reaction.[Wait=500] Why do you think you and the original behind this call have the same voice?[Color=White][Wait=500][Space=2]
+[Color=Yellow]Didn't it strike you that he was the only contact on this phone?[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Yellow]I'm telling you the truth.[Wait=500] It might seem troubling, but you have to accept that you're just a mere reproduction.[Color=White][Wait=500][Space=2]
+[Color=Yellow]But why would it matter?[Wait=500] You're now the perfect subject I was waiting for.[Color=White][Wait=500][Space=2]
+...[Wait=500] What do you mean by...[Wait=500] The perfect subject?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Yellow]Not all.[Wait=500] I just said that you were subject 835.[Wait=500] Three are still alive to this day.[Color=White][Wait=500][Space=2]
+[Color=Yellow]One was not able to handle the virus. However, he managed to take out his tracker and is still roaming outside.[Color=White][Wait=500][Space=2]
+[Color=Yellow]He was responsible for the death of some clones because of his hostility.[Color=White][Wait=500][Space=2]
+[Color=Yellow]The other one was immune, but he managed to bypass my security and free himself.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Yellow]Oh?[Wait=500] He contacted you?[Wait=500] How curious. This must mean he's still on the island.[Color=White][Wait=500][Space=2]
+[Color=Magenta][Beep=True]DoN[Wait=500][Beep=True]'t tRu[Wait=500][Beep=True]st hIm[Wait=500][Beep=True]. aLl oF[Wait=500][Beep=True] tHeSe dEa[Wait=500][Beep=True]tHs iS[Wait=500][Beep=True] bEcAuSe[Wait=500][Beep=True] oF hIm.[Color=White][Wait=500][Space=2]
+...[Wait=500] I can't believe all that...[Wait=500] Why am I here?[Wait=500] TELL ME WHY DID YOU MAKE ME?![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Yellow]I understand your confusion.[Wait=500] But the survival of humankind is at stake at this very moment.[Color=White][Wait=500][Space=2]
+[Color=Yellow]A virus is spreading, and it's undetectable.[Wait=500] I call it the Emotoxin.[Wait=500] No one believed me.[Color=White][Wait=500][Space=2]
+[Color=Yellow]It amplifies the intensity of our emotions, causing us to burst into rage, euphoria, or misery.[Color=White][Wait=500][Space=2]
+...[Wait=500] And in what way could this cause the end of humankind?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Yellow]You should see how an infected acts.[Color=White][Wait=500][Space=2]
+[Color=Yellow]In our world filled with hate, it would cause people to kill each other over a small argument.[Color=White][Wait=500][Space=2]
+...[Wait=500] I'm not infected, right?[Wait=500] So why would you do all that in the first place?[Wait=500][Space=2]
+Why not use a lab rat instead of killing HUNDREDS OF HUMANS![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Yellow]The Emotoxin only affects humans. So I preferred to base my research on clones instead of real humans.[Color=White][Wait=500][Space=2]
+[Color=Yellow]I chose to clone you because your DNA was highly compatible with cloning and resistant to the Emotoxin structure.[Color=White][Wait=500][Space=2]
+[Color=Yellow]All these puzzles were tests to see if you were affected by the toxin by playing with your emotions.[Color=White][Wait=500][Space=2]
+[Color=Yellow]I think it might be time to get out of this room now.[Wait=500] I need your blood.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Y-Yes![Wait=500] I'M STAYING INSIDE, YOU PSYCHOPATH![Wait=500][Space=2]
+I'M NOT GOING TO LET YOU SUCK MY BLOOD![Wait=500] I MAY BE A CLONE, BUT I'M NOT BELIEVING ALL THIS SHIT![Wait=500][Space=2]
+[Color=Yellow]...[Wait=500] Hmmm...[Wait=500] Unfortunately for you, I anticipated this kind of reaction.[Color=White][Wait=500][Space=2]
+[Color=Yellow]What are your last words?[Color=White][Wait=500][Space=2]
+Y-You're bluffing![Wait=500] I'm not going to fall for this eith-[Color=Gray]*PSHHHHHHHHHH*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500] OH SHIT![Wait=500] THERE'S GREEN GAS SPREADING IN THE ROOM![Wait=500][Space=2]
+[Color=Gray]*Door shake*[Color=White]...[Wait=500][Space=2]
+LET ME OUT, THIS FUCKER LOCKED THE DOOR![Wait=500][Space=2]
+[Color=Yellow]You made your own choices, you and your friend.[Wait=500] Now you'll have to accept the consequences.[Color=White][Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White]... No...[Wait=500] [Color=Gray]*Cough*[Color=White] [Color=Gray]*Cough*[Color=White]...[Wait=500][Space=2]
+.[Wait=500].[Wait=500].[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>N-NO![Wait=500] I WON'T FOLLOW HIM![Wait=500][Space=2]
+I DON'T TRUST YOU ANYMORE![Wait=500] You were plotting with him since the beginning, right?[Wait=500][Space=2]
+[Color=Gray]*SLAM*[Color=White] OUCH![Wait=500] I'M GETTING OUT OF HERE![Wait=500][Space=2]
+[Color=Gray]*Fast footsteps*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>LIAR![Wait=500][Space=2]
+You could be behind THIS DOOR [Color=Gray]*SLAM*[Color=White]...[Wait=500][Space=2]
+THIS DOOR [Color=Gray]*SLAM*[Color=White]...[Wait=500][Space=2]
+...[Wait=500] Ah AH! Just as I thought, a monitoring room![Wait=500][Space=2]
+You were here before, huh?[Wait=500] Planning for the next puzzle and acting as if you were discovering it with me.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>You're the crazy one here, cloning yourself and watching you suffer with this mad scientist![Wait=500][Space=2]
+...[Wait=500] Oh![Wait=500] Look![Wait=500] How unfortunate for you![Wait=500][Space=2]
+"This button should only be used in case that the Emotoxin breaches out.[Wait=500][Space=2]
+The explosion will eradicate all living organisms in a 5 kilometers radius."[Wait=500][Space=2]
+...[Wait=500] You really put a self-destruct button here?[Wait=500] Too bad, because I'm going to press it.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>AND I WILL ALSO KILL YOU AND YOUR SCIENTIST FRIEND![Wait=500][Space=2]
+I will end this whole madness![Wait=500] Hundreds of different versions of you were killed.[Wait=500] THEY HAD FEELINGS, YOU KNOW?![Wait=500][Space=2]
+I'm willing to sacrifice, as revenge for all the ones that suffered before me.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500] Is it really for the survival of humanity?[Wait=500] It's not a trick so that I get out and you can shoot me easily?[Wait=500][Space=2]
+[Color=Yellow]Absolutely not.[Wait=500] I care for my research, and I wouldn't waste any of my bullets or any of your blood.[Color=White][Wait=500][Space=2]
+...[Wait=500] [Color=Gray]*Door opening*[Color=White]...[Wait=500] [Color=Yellow]So you opened.[Color=White][Wait=500][Space=2]
+I don't know what you mean by needing my blood, but I assume this will not be pleasurable?[Wait=500][Space=2]
+[Color=Yellow]You guessed it. But I will do what's possible to keep you alive after that.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Yellow]Good.[Wait=500] Now, original, you'll excuse us, but we have to end the call here.[Wait=500] I have to borrow this clone.[Color=White][Wait=500][Space=2]
+W-Wait... I have a question.[Wait=500] Why did you make us contact each other?[Wait=500][Space=2]
+[Color=Yellow]I needed a full panel of your emotions right when I knew that you were the right one.[Color=White][Wait=500][Space=2]
+[Color=Yellow]There was no better option than using yourself to stimulate every aspect of your personality.[Color=White][Wait=500][Space=2]
+[Color=Yellow]Talking to yourself shows how human behavior is not absolute for a single person.[Color=White][Wait=500][Space=2]
+[Color=Yellow]The gap between what we think we'd do and what we actually do is indeterminable.[Color=White][Wait=500][Space=2]
+[Color=Yellow]By calling the original, you could explore every aspect of yourself...[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Yellow]I'm a scientist, not a social expert.[Wait=500] Now, original, we have to end the call here.[Wait=500] I have to borrow this clone.[Color=White][Wait=500][Space=2]
+W-Wait... I have a question.[Wait=500] Why did you make us contact each other?[Wait=500][Space=2]
+[Color=Yellow]I needed a full panel of your emotions right when I knew that you were the right one.[Color=White][Wait=500][Space=2]
+[Color=Yellow]There was no better option than using yourself to stimulate every aspect of your personality.[Color=White][Wait=500][Space=2]
+[Color=Yellow]Talking to yourself shows how human behavior is not absolute for a single person.[Color=White][Wait=500][Space=2]
+[Color=Yellow]The gap between what we think we'd do and what we actually do is indeterminable.[Color=White][Wait=500][Space=2]
+[Color=Yellow]By calling the original, you could explore every aspect of yourself...[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Yellow]Confusing, I know.[Wait=500] Even if I simplify the terms, it's still a concept most won't understand.[Color=White][Wait=500][Space=2]
+...[Wait=500][Space=2]
+One more thing.[Wait=500] Can I talk one last time with the original?[Wait=500][Space=2]
+[Color=Yellow]Go on.[Wait=500] I've waited years for you to exist, so I can wait one more minute.[Color=White][Wait=500][Space=2]
+...[Wait=500] Hey...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>You bet it was![Wait=500] That's unfortunate that we have to end on this "save the humanity" tone...[Wait=500][Space=2]
+But I guess we can't do anything about it.[Wait=500][Space=2]
+The world chose you to be immune.[Wait=500] And by you, that includes me...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Ahah![Wait=500] I guess you're right![Wait=500][Space=2]
+...[Wait=500] Thank you for staying with me...[Wait=500] I know I was just a random call of a stranger at the beginning, but...[Wait=500][Space=2]
+But I hope I'll be able to call you again one day.[Wait=500] We'll be able to eat something at your favorite restaurant![Wait=500][Space=2]
+I know which one it is since I've got the same memories as you, eheh![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Ahahah![Wait=500] That's tru-.[Wait=500][Space=2]
+[Color=Yellow]We have to go.[Color=White][Wait=500][Space=2]
+O-Oh...[Wait=500] Well, I guess it's a goodbye.[Wait=500][Space=2]
+I really hope to see you again.[Wait=500] Until then, believe in yourself.[Wait=500] I know we're great people.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=3][Content=Small?]]
+[Choice2=[NextScene=4][Content=Well-preserved?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=5][TrustAdd=25][Content=Nah. Why would someone want to clean an old museum anyway? It's just a coincidence.]]
+[Choice2=[NextScene=6][Content=I guess there is. Why would it be cleaner than the other buildings otherwise?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=6][Content=You're afraid of seeing someone now?]]
+[Choice2=[NextScene=7][TrustAdd=-25][Content=Well, don't enter it then.]]
+[Choice3=[NextScene=8][Content=Sorry to say this, but it doesn't seem like you have a choice...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=8][TrustAdd=25][Content=Everything's gonna be fine as long as we work together.]]
+[Choice2=[NextScene=9][TrustAdd=-25][Content=I knew it! You're chicken-hearted!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=Is there something weird in there?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=12][TrustAdd=25][Content=Well... I am.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=6][Content=You're afraid of seeing someone now?]]
+[Choice2=[NextScene=7][TrustAdd=-25][Content=Well, don't enter it then.]]
+[Choice3=[NextScene=8][Content=Sorry to say this, but it doesn't seem like you have the choice...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=15][Content=So? What’s inside?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=16][Content=That’s weird...]]
+[Choice2=[NextScene=17][TrustAdd=-25][Content=That’s so cool!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=18][TrustAdd=-25][Content=You're becoming paranoid?]]
+[Choice2=[NextScene=19][Content=Someone’s living here?]]
+[Choice3=[NextScene=20][TrustAdd=25][Content=That means we have a new mystery to solve!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=18][TrustAdd=-25][Content=You're definitely becoming paranoid.]]
+[Choice2=[NextScene=19][Content=Is... someone living here?]]
+[Choice3=[NextScene=20][TrustAdd=25][Content=Seems like we’ll have to solve this mystery together!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=21][TrustAdd=-25][Content=I think I’d be braver than you!]]
+[Choice2=[NextScene=22][TrustAdd=25][Content=I think I’d manage things like you.]]
+[Choice3=[NextScene=23][Content=I’d be... more fearful than you!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=24][TrustAdd=25][Content=Calm down. That doesn’t justify any panic.]]
+[Choice2=[NextScene=25][TrustAdd=-25][Content=Don’t throw up on the art, please.]]
+[Choice3=[NextScene=26][TrustAdd=-25][Content=I was joking! There’s surely no one here.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=27][Content=What’s around you again?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=28][Content=Go and see the paintings.]]
+[Choice2=[NextScene=29][Content=Go and see the sculpture.]]
+[Choice3=[NextScene=30][Content=Go and see the inscriptions on the rock.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=31][Content=Is there something else besides art here?]]
+[Choice2=[NextScene=39][Content=Can you describe it more precisely?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=31][Content=Is there something else besides art here?]]
+[Choice2=[NextScene=40][Content=Can you describe it more precisely?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=31][Content=Is there something else besides art here?]]
+[Choice2=[NextScene=41][Content=Can you describe it more precisely?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=32][Content=What’s going on?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=55][TrustAdd=25][Content=Of course! I will be with you until the end.]]
+[Choice2=[NextScene=56][TrustAdd=-25][Content=Uhm, I have more alluring stuff to do.]]
+[Choice3=[NextScene=57][TrustAdd=25][Content=Sorry, but I don't feel comfortable hearing someone slowly dying on the phone...]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=59][TrustAdd=-25][Content=But they'll be hostile!]]
+[Choice2=[NextScene=60][Content=Maybe we can make a deal so they free you.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=64][Content=Where are you now?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=62][TrustAdd=-25][Content=I would go back and search for another way out if I were you.]]
+[Choice2=[NextScene=63][Content=Do whatever you want, it's your responsibility.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=66][Content=Can you hear me?]]
+[Choice2=[NextScene=66][Content=I'm still here!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=92][Content=DON'T GIVE UP!]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=106][Content=We'll go and see a movie too! Since your favorites are also mine.]]
 [Choice2=[NextScene=106][Content=I hope you don't remember the awkward ones...]]</t>
-  </si>
-  <si>
-    <t>[Choice1=[NextScene=107][Content=See you later.]]</t>
   </si>
 </sst>
 </file>
@@ -3689,8 +3696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="E37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView topLeftCell="E52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="120" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3736,7 +3743,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>188</v>
+        <v>125</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>29</v>
@@ -3752,7 +3759,7 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>210</v>
+        <v>242</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>12</v>
@@ -3768,10 +3775,10 @@
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>205</v>
+        <v>130</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>299</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3782,7 +3789,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>209</v>
+        <v>243</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>26</v>
@@ -3796,7 +3803,7 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>211</v>
+        <v>133</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>27</v>
@@ -3812,7 +3819,7 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>30</v>
@@ -3828,7 +3835,7 @@
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>212</v>
+        <v>134</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>33</v>
@@ -3856,7 +3863,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>213</v>
+        <v>135</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>32</v>
@@ -3870,10 +3877,10 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>214</v>
+        <v>244</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>215</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3884,7 +3891,7 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>216</v>
+        <v>137</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>34</v>
@@ -3898,7 +3905,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>35</v>
@@ -3915,7 +3922,7 @@
         <v>19</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>217</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -3926,7 +3933,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>218</v>
+        <v>139</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>36</v>
@@ -3971,7 +3978,7 @@
         <v>21</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>219</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4024,7 +4031,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>220</v>
+        <v>141</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>52</v>
@@ -4040,7 +4047,7 @@
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>53</v>
@@ -4056,10 +4063,10 @@
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>222</v>
+        <v>142</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>299</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4088,10 +4095,10 @@
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>223</v>
+        <v>143</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>299</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4102,7 +4109,7 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>224</v>
+        <v>144</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>41</v>
@@ -4118,7 +4125,7 @@
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>225</v>
+        <v>145</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>42</v>
@@ -4132,7 +4139,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>226</v>
+        <v>146</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>54</v>
@@ -4146,7 +4153,7 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>227</v>
+        <v>147</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>55</v>
@@ -4160,7 +4167,7 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>56</v>
@@ -4174,7 +4181,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>57</v>
@@ -4188,7 +4195,7 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>58</v>
@@ -4202,7 +4209,7 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>228</v>
+        <v>148</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>59</v>
@@ -4216,7 +4223,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>229</v>
+        <v>149</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>60</v>
@@ -4230,7 +4237,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>61</v>
@@ -4246,7 +4253,7 @@
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>230</v>
+        <v>150</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>62</v>
@@ -4262,7 +4269,7 @@
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>231</v>
+        <v>151</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>63</v>
@@ -4276,7 +4283,7 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="8" t="s">
-        <v>232</v>
+        <v>152</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>43</v>
@@ -4290,7 +4297,7 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>234</v>
+        <v>154</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>64</v>
@@ -4304,7 +4311,7 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>233</v>
+        <v>153</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>65</v>
@@ -4318,7 +4325,7 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>235</v>
+        <v>155</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>66</v>
@@ -4332,7 +4339,7 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>236</v>
+        <v>156</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>44</v>
@@ -4346,7 +4353,7 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>237</v>
+        <v>157</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>44</v>
@@ -4360,7 +4367,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>238</v>
+        <v>158</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>45</v>
@@ -4374,7 +4381,7 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>239</v>
+        <v>159</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>67</v>
@@ -4388,7 +4395,7 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>240</v>
+        <v>160</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>68</v>
@@ -4402,7 +4409,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>69</v>
@@ -4416,7 +4423,7 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>241</v>
+        <v>161</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>70</v>
@@ -4430,7 +4437,7 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>242</v>
+        <v>162</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>71</v>
@@ -4444,7 +4451,7 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>243</v>
+        <v>163</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>46</v>
@@ -4458,7 +4465,7 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>258</v>
+        <v>178</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>72</v>
@@ -4492,7 +4499,7 @@
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>48</v>
@@ -4508,10 +4515,10 @@
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>206</v>
+        <v>288</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>299</v>
+        <v>200</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4540,7 +4547,7 @@
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>244</v>
+        <v>164</v>
       </c>
       <c r="F57" s="8" t="s">
         <v>73</v>
@@ -4554,7 +4561,7 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>50</v>
@@ -4568,7 +4575,7 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="F59" s="8" t="s">
         <v>74</v>
@@ -4582,7 +4589,7 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8" t="s">
-        <v>245</v>
+        <v>165</v>
       </c>
       <c r="F60" s="8" t="s">
         <v>75</v>
@@ -4596,7 +4603,7 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>246</v>
+        <v>166</v>
       </c>
       <c r="F61" s="8" t="s">
         <v>76</v>
@@ -4610,7 +4617,7 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="8" t="s">
-        <v>247</v>
+        <v>167</v>
       </c>
       <c r="F62" s="8" t="s">
         <v>51</v>
@@ -4624,7 +4631,7 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>248</v>
+        <v>168</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>77</v>
@@ -4638,7 +4645,7 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>249</v>
+        <v>169</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>78</v>
@@ -4652,7 +4659,7 @@
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>250</v>
+        <v>170</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>79</v>
@@ -4666,7 +4673,7 @@
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>251</v>
+        <v>171</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>80</v>
@@ -4696,7 +4703,7 @@
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>252</v>
+        <v>172</v>
       </c>
       <c r="F68" s="8" t="s">
         <v>82</v>
@@ -4712,7 +4719,7 @@
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>253</v>
+        <v>173</v>
       </c>
       <c r="F69" s="8" t="s">
         <v>83</v>
@@ -4726,7 +4733,7 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>254</v>
+        <v>174</v>
       </c>
       <c r="F70" s="8" t="s">
         <v>84</v>
@@ -4740,7 +4747,7 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="8" t="s">
-        <v>255</v>
+        <v>175</v>
       </c>
       <c r="F71" s="8" t="s">
         <v>86</v>
@@ -4754,7 +4761,7 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="8" t="s">
-        <v>256</v>
+        <v>176</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>85</v>
@@ -4770,7 +4777,7 @@
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="8" t="s">
-        <v>257</v>
+        <v>177</v>
       </c>
       <c r="F73" s="8" t="s">
         <v>87</v>
@@ -4803,8 +4810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305A82C4-79AC-4307-9167-395B8B5B112C}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F109" sqref="F109"/>
+    <sheetView tabSelected="1" topLeftCell="F103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I107" sqref="I107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="120" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4846,10 +4853,10 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>94</v>
+        <v>246</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>208</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4860,10 +4867,10 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>95</v>
+        <v>247</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>259</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4874,10 +4881,10 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>260</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4888,10 +4895,10 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>97</v>
+        <v>248</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>261</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4902,10 +4909,10 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>98</v>
+        <v>249</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>262</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4916,10 +4923,10 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>99</v>
+        <v>250</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>263</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4930,10 +4937,10 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>100</v>
+        <v>251</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>264</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4944,10 +4951,10 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>265</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4958,10 +4965,10 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>145</v>
+        <v>252</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>266</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4972,10 +4979,10 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>101</v>
+        <v>253</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>267</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -4986,10 +4993,10 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>146</v>
+        <v>254</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>268</v>
+        <v>329</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5000,10 +5007,10 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>102</v>
+        <v>255</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>269</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5014,10 +5021,10 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8" t="s">
-        <v>103</v>
+        <v>256</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>270</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5028,10 +5035,10 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>147</v>
+        <v>257</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>271</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5042,10 +5049,10 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>104</v>
+        <v>258</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>272</v>
+        <v>332</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5056,10 +5063,10 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>105</v>
+        <v>259</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>273</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5070,10 +5077,10 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>106</v>
+        <v>260</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>274</v>
+        <v>334</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5084,10 +5091,10 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>107</v>
+        <v>261</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>275</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5098,10 +5105,10 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>148</v>
+        <v>262</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>276</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5112,10 +5119,10 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>108</v>
+        <v>263</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>277</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5126,10 +5133,10 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>109</v>
+        <v>264</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>277</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5140,10 +5147,10 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>110</v>
+        <v>265</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>277</v>
+        <v>337</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5154,10 +5161,10 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>111</v>
+        <v>266</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>277</v>
+        <v>337</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5168,10 +5175,10 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8" t="s">
-        <v>149</v>
+        <v>267</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>277</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5182,10 +5189,10 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>150</v>
+        <v>268</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>277</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5196,10 +5203,10 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>112</v>
+        <v>269</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>277</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5210,10 +5217,10 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>113</v>
+        <v>270</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>278</v>
+        <v>338</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5224,10 +5231,10 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>151</v>
+        <v>271</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>279</v>
+        <v>339</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5238,10 +5245,10 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>152</v>
+        <v>272</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>280</v>
+        <v>340</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5252,10 +5259,10 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8" t="s">
-        <v>153</v>
+        <v>273</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>281</v>
+        <v>341</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5266,10 +5273,10 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>154</v>
+        <v>274</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>282</v>
+        <v>342</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5280,10 +5287,10 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>114</v>
+        <v>275</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>283</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5294,10 +5301,10 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>155</v>
+        <v>276</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>284</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5308,10 +5315,10 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>156</v>
+        <v>277</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>285</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5322,10 +5329,10 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>117</v>
+        <v>278</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>286</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5336,10 +5343,10 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>151</v>
+        <v>271</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>287</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5350,10 +5357,10 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>152</v>
+        <v>272</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>288</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5364,10 +5371,10 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="8" t="s">
-        <v>153</v>
+        <v>273</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>289</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5378,10 +5385,10 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>118</v>
+        <v>279</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>290</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5392,10 +5399,10 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>119</v>
+        <v>280</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>290</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5406,10 +5413,10 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>290</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5420,10 +5427,10 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>118</v>
+        <v>281</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>291</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5434,10 +5441,10 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>119</v>
+        <v>282</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>291</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5448,10 +5455,10 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>291</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5462,10 +5469,10 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>120</v>
+        <v>283</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>292</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5476,10 +5483,10 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>293</v>
+        <v>194</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5490,10 +5497,10 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>158</v>
+        <v>284</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>294</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5504,10 +5511,10 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>295</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5520,10 +5527,10 @@
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>296</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5536,10 +5543,10 @@
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>162</v>
+        <v>285</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>297</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5552,10 +5559,10 @@
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>204</v>
+        <v>286</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>298</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5566,10 +5573,10 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>300</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5580,10 +5587,10 @@
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>122</v>
+        <v>287</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>301</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5594,10 +5601,10 @@
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>123</v>
+        <v>289</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>302</v>
+        <v>343</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5608,10 +5615,10 @@
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="8" t="s">
-        <v>124</v>
+        <v>290</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>303</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5622,10 +5629,10 @@
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>125</v>
+        <v>291</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>304</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5636,10 +5643,10 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>126</v>
+        <v>292</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>305</v>
+        <v>204</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5650,10 +5657,10 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>127</v>
+        <v>293</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>306</v>
+        <v>344</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5664,10 +5671,10 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>307</v>
+        <v>345</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5678,10 +5685,10 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>129</v>
+        <v>294</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>307</v>
+        <v>345</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5692,10 +5699,10 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="8" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>308</v>
+        <v>346</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5706,10 +5713,10 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>131</v>
+        <v>295</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>309</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5720,10 +5727,10 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>310</v>
+        <v>206</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5736,10 +5743,10 @@
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>164</v>
+        <v>296</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>311</v>
+        <v>207</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5752,10 +5759,10 @@
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>165</v>
+        <v>116</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>312</v>
+        <v>347</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5766,10 +5773,10 @@
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>175</v>
+        <v>118</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>313</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5780,10 +5787,10 @@
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>176</v>
+        <v>119</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>314</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5794,10 +5801,10 @@
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>177</v>
+        <v>120</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>315</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5808,10 +5815,10 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>178</v>
+        <v>121</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>316</v>
+        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5824,10 +5831,10 @@
         <v>7</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>179</v>
+        <v>122</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>317</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5840,10 +5847,10 @@
         <v>7</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>180</v>
+        <v>123</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>318</v>
+        <v>213</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5856,10 +5863,10 @@
         <v>7</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>181</v>
+        <v>124</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>319</v>
+        <v>214</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5870,10 +5877,10 @@
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="13" t="s">
-        <v>182</v>
+        <v>297</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>320</v>
+        <v>215</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5886,10 +5893,10 @@
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="8" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>321</v>
+        <v>216</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5900,10 +5907,10 @@
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
       <c r="E76" s="8" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>322</v>
+        <v>217</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5914,10 +5921,10 @@
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
       <c r="E77" s="8" t="s">
-        <v>134</v>
+        <v>298</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>322</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5928,10 +5935,10 @@
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
       <c r="E78" s="13" t="s">
-        <v>136</v>
+        <v>299</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>322</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5942,10 +5949,10 @@
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
       <c r="E79" s="13" t="s">
-        <v>166</v>
+        <v>300</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>323</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5956,10 +5963,10 @@
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
       <c r="E80" s="13" t="s">
-        <v>167</v>
+        <v>301</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>324</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5970,10 +5977,10 @@
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
       <c r="E81" s="13" t="s">
-        <v>168</v>
+        <v>302</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>325</v>
+        <v>220</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5984,10 +5991,10 @@
       <c r="C82" s="12"/>
       <c r="D82" s="12"/>
       <c r="E82" s="13" t="s">
-        <v>169</v>
+        <v>303</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>326</v>
+        <v>221</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -5998,10 +6005,10 @@
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
       <c r="E83" s="13" t="s">
-        <v>170</v>
+        <v>304</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>327</v>
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6012,10 +6019,10 @@
       <c r="C84" s="12"/>
       <c r="D84" s="12"/>
       <c r="E84" s="13" t="s">
-        <v>171</v>
+        <v>305</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>328</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6026,10 +6033,10 @@
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
       <c r="E85" s="13" t="s">
-        <v>172</v>
+        <v>117</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>329</v>
+        <v>224</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6040,10 +6047,10 @@
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
       <c r="E86" s="13" t="s">
-        <v>173</v>
+        <v>306</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>330</v>
+        <v>225</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6054,10 +6061,10 @@
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
       <c r="E87" s="13" t="s">
-        <v>174</v>
+        <v>307</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>331</v>
+        <v>226</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6068,10 +6075,10 @@
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
       <c r="E88" s="13" t="s">
-        <v>183</v>
+        <v>308</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>332</v>
+        <v>227</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6082,10 +6089,10 @@
       <c r="C89" s="12"/>
       <c r="D89" s="12"/>
       <c r="E89" s="13" t="s">
-        <v>184</v>
+        <v>309</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>333</v>
+        <v>228</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6096,10 +6103,10 @@
       <c r="C90" s="12"/>
       <c r="D90" s="12"/>
       <c r="E90" s="13" t="s">
-        <v>185</v>
+        <v>310</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>334</v>
+        <v>229</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6112,10 +6119,10 @@
       </c>
       <c r="D91" s="12"/>
       <c r="E91" s="13" t="s">
-        <v>186</v>
+        <v>311</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>335</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6128,10 +6135,10 @@
       </c>
       <c r="D92" s="12"/>
       <c r="E92" s="13" t="s">
-        <v>187</v>
+        <v>312</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6144,10 +6151,10 @@
       </c>
       <c r="D93" s="12"/>
       <c r="E93" s="13" t="s">
-        <v>203</v>
+        <v>129</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>298</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6160,10 +6167,10 @@
       </c>
       <c r="D94" s="12"/>
       <c r="E94" s="13" t="s">
-        <v>189</v>
+        <v>313</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>337</v>
+        <v>231</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6174,10 +6181,10 @@
       <c r="C95" s="12"/>
       <c r="D95" s="12"/>
       <c r="E95" s="13" t="s">
-        <v>190</v>
+        <v>126</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>338</v>
+        <v>232</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6188,10 +6195,10 @@
       <c r="C96" s="12"/>
       <c r="D96" s="12"/>
       <c r="E96" s="13" t="s">
-        <v>191</v>
+        <v>314</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>339</v>
+        <v>233</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6202,10 +6209,10 @@
       <c r="C97" s="12"/>
       <c r="D97" s="12"/>
       <c r="E97" s="13" t="s">
-        <v>192</v>
+        <v>315</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>340</v>
+        <v>234</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6216,10 +6223,10 @@
       <c r="C98" s="12"/>
       <c r="D98" s="12"/>
       <c r="E98" s="13" t="s">
-        <v>193</v>
+        <v>316</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>341</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6232,10 +6239,10 @@
       </c>
       <c r="D99" s="12"/>
       <c r="E99" s="13" t="s">
-        <v>194</v>
+        <v>127</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>342</v>
+        <v>236</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6248,10 +6255,10 @@
       </c>
       <c r="D100" s="12"/>
       <c r="E100" s="13" t="s">
-        <v>202</v>
+        <v>128</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>298</v>
+        <v>199</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6264,10 +6271,10 @@
       </c>
       <c r="D101" s="12"/>
       <c r="E101" s="13" t="s">
-        <v>195</v>
+        <v>317</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>343</v>
+        <v>237</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6278,10 +6285,10 @@
       <c r="C102" s="12"/>
       <c r="D102" s="12"/>
       <c r="E102" s="13" t="s">
-        <v>197</v>
+        <v>318</v>
       </c>
       <c r="F102" s="13" t="s">
-        <v>344</v>
+        <v>238</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6292,10 +6299,10 @@
       <c r="C103" s="12"/>
       <c r="D103" s="12"/>
       <c r="E103" s="13" t="s">
-        <v>196</v>
+        <v>319</v>
       </c>
       <c r="F103" s="13" t="s">
-        <v>344</v>
+        <v>238</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6306,10 +6313,10 @@
       <c r="C104" s="12"/>
       <c r="D104" s="12"/>
       <c r="E104" s="13" t="s">
-        <v>198</v>
+        <v>320</v>
       </c>
       <c r="F104" s="13" t="s">
-        <v>345</v>
+        <v>239</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6320,10 +6327,10 @@
       <c r="C105" s="12"/>
       <c r="D105" s="12"/>
       <c r="E105" s="13" t="s">
-        <v>199</v>
+        <v>321</v>
       </c>
       <c r="F105" s="13" t="s">
-        <v>346</v>
+        <v>240</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6334,10 +6341,10 @@
       <c r="C106" s="12"/>
       <c r="D106" s="12"/>
       <c r="E106" s="13" t="s">
-        <v>200</v>
+        <v>322</v>
       </c>
       <c r="F106" s="13" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6348,10 +6355,10 @@
       <c r="C107" s="12"/>
       <c r="D107" s="12"/>
       <c r="E107" s="13" t="s">
-        <v>201</v>
+        <v>323</v>
       </c>
       <c r="F107" s="13" t="s">
-        <v>348</v>
+        <v>241</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6360,14 +6367,14 @@
       </c>
       <c r="B108" s="11"/>
       <c r="C108" s="12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D108" s="12"/>
       <c r="E108" s="13" t="s">
-        <v>207</v>
+        <v>131</v>
       </c>
       <c r="F108" s="13" t="s">
-        <v>298</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>